<commit_message>
CCMY new additional scene_types(before/after)
</commit_message>
<xml_diff>
--- a/Projects/CCMY/Data/Template.xlsx
+++ b/Projects/CCMY/Data/Template.xlsx
@@ -12,27 +12,30 @@
     <sheet name="Availability" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$2:$E$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$B$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$B$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$B$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$B$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$B$1:$K$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$B$1:$K$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$2:$E$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="102">
   <si>
     <t xml:space="preserve">Store Type</t>
   </si>
@@ -128,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve">CCRM Cooler Total Number of Shelves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCRM Cooler (Before)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCRM Cooler (After)</t>
   </si>
   <si>
     <t xml:space="preserve">Retailer Cooler Shelf  - 8 -15 facing</t>
@@ -356,7 +365,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -379,8 +388,14 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -393,7 +408,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -417,6 +432,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -431,14 +453,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFF66"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF66"/>
       </patternFill>
     </fill>
     <fill>
@@ -518,7 +540,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -528,7 +550,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,59 +562,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -600,11 +622,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -620,7 +642,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -628,11 +650,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -857,30 +879,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:15"/>
+  <dimension ref="1:18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1023" min="12" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1926,6 +1947,7 @@
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
@@ -2959,6 +2981,7 @@
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
@@ -4002,6 +4025,7 @@
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -5045,6 +5069,7 @@
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
@@ -6088,6 +6113,7 @@
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
@@ -7131,6 +7157,7 @@
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
@@ -8174,6 +8201,7 @@
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
@@ -9215,8 +9243,9 @@
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
+      <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>25</v>
@@ -9242,9 +9271,1021 @@
         <v>0</v>
       </c>
       <c r="K9" s="7"/>
-      <c r="AMJ9" s="10"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="Z9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="0"/>
+      <c r="AC9" s="0"/>
+      <c r="AD9" s="0"/>
+      <c r="AE9" s="0"/>
+      <c r="AF9" s="0"/>
+      <c r="AG9" s="0"/>
+      <c r="AH9" s="0"/>
+      <c r="AI9" s="0"/>
+      <c r="AJ9" s="0"/>
+      <c r="AK9" s="0"/>
+      <c r="AL9" s="0"/>
+      <c r="AM9" s="0"/>
+      <c r="AN9" s="0"/>
+      <c r="AO9" s="0"/>
+      <c r="AP9" s="0"/>
+      <c r="AQ9" s="0"/>
+      <c r="AR9" s="0"/>
+      <c r="AS9" s="0"/>
+      <c r="AT9" s="0"/>
+      <c r="AU9" s="0"/>
+      <c r="AV9" s="0"/>
+      <c r="AW9" s="0"/>
+      <c r="AX9" s="0"/>
+      <c r="AY9" s="0"/>
+      <c r="AZ9" s="0"/>
+      <c r="BA9" s="0"/>
+      <c r="BB9" s="0"/>
+      <c r="BC9" s="0"/>
+      <c r="BD9" s="0"/>
+      <c r="BE9" s="0"/>
+      <c r="BF9" s="0"/>
+      <c r="BG9" s="0"/>
+      <c r="BH9" s="0"/>
+      <c r="BI9" s="0"/>
+      <c r="BJ9" s="0"/>
+      <c r="BK9" s="0"/>
+      <c r="BL9" s="0"/>
+      <c r="BM9" s="0"/>
+      <c r="BN9" s="0"/>
+      <c r="BO9" s="0"/>
+      <c r="BP9" s="0"/>
+      <c r="BQ9" s="0"/>
+      <c r="BR9" s="0"/>
+      <c r="BS9" s="0"/>
+      <c r="BT9" s="0"/>
+      <c r="BU9" s="0"/>
+      <c r="BV9" s="0"/>
+      <c r="BW9" s="0"/>
+      <c r="BX9" s="0"/>
+      <c r="BY9" s="0"/>
+      <c r="BZ9" s="0"/>
+      <c r="CA9" s="0"/>
+      <c r="CB9" s="0"/>
+      <c r="CC9" s="0"/>
+      <c r="CD9" s="0"/>
+      <c r="CE9" s="0"/>
+      <c r="CF9" s="0"/>
+      <c r="CG9" s="0"/>
+      <c r="CH9" s="0"/>
+      <c r="CI9" s="0"/>
+      <c r="CJ9" s="0"/>
+      <c r="CK9" s="0"/>
+      <c r="CL9" s="0"/>
+      <c r="CM9" s="0"/>
+      <c r="CN9" s="0"/>
+      <c r="CO9" s="0"/>
+      <c r="CP9" s="0"/>
+      <c r="CQ9" s="0"/>
+      <c r="CR9" s="0"/>
+      <c r="CS9" s="0"/>
+      <c r="CT9" s="0"/>
+      <c r="CU9" s="0"/>
+      <c r="CV9" s="0"/>
+      <c r="CW9" s="0"/>
+      <c r="CX9" s="0"/>
+      <c r="CY9" s="0"/>
+      <c r="CZ9" s="0"/>
+      <c r="DA9" s="0"/>
+      <c r="DB9" s="0"/>
+      <c r="DC9" s="0"/>
+      <c r="DD9" s="0"/>
+      <c r="DE9" s="0"/>
+      <c r="DF9" s="0"/>
+      <c r="DG9" s="0"/>
+      <c r="DH9" s="0"/>
+      <c r="DI9" s="0"/>
+      <c r="DJ9" s="0"/>
+      <c r="DK9" s="0"/>
+      <c r="DL9" s="0"/>
+      <c r="DM9" s="0"/>
+      <c r="DN9" s="0"/>
+      <c r="DO9" s="0"/>
+      <c r="DP9" s="0"/>
+      <c r="DQ9" s="0"/>
+      <c r="DR9" s="0"/>
+      <c r="DS9" s="0"/>
+      <c r="DT9" s="0"/>
+      <c r="DU9" s="0"/>
+      <c r="DV9" s="0"/>
+      <c r="DW9" s="0"/>
+      <c r="DX9" s="0"/>
+      <c r="DY9" s="0"/>
+      <c r="DZ9" s="0"/>
+      <c r="EA9" s="0"/>
+      <c r="EB9" s="0"/>
+      <c r="EC9" s="0"/>
+      <c r="ED9" s="0"/>
+      <c r="EE9" s="0"/>
+      <c r="EF9" s="0"/>
+      <c r="EG9" s="0"/>
+      <c r="EH9" s="0"/>
+      <c r="EI9" s="0"/>
+      <c r="EJ9" s="0"/>
+      <c r="EK9" s="0"/>
+      <c r="EL9" s="0"/>
+      <c r="EM9" s="0"/>
+      <c r="EN9" s="0"/>
+      <c r="EO9" s="0"/>
+      <c r="EP9" s="0"/>
+      <c r="EQ9" s="0"/>
+      <c r="ER9" s="0"/>
+      <c r="ES9" s="0"/>
+      <c r="ET9" s="0"/>
+      <c r="EU9" s="0"/>
+      <c r="EV9" s="0"/>
+      <c r="EW9" s="0"/>
+      <c r="EX9" s="0"/>
+      <c r="EY9" s="0"/>
+      <c r="EZ9" s="0"/>
+      <c r="FA9" s="0"/>
+      <c r="FB9" s="0"/>
+      <c r="FC9" s="0"/>
+      <c r="FD9" s="0"/>
+      <c r="FE9" s="0"/>
+      <c r="FF9" s="0"/>
+      <c r="FG9" s="0"/>
+      <c r="FH9" s="0"/>
+      <c r="FI9" s="0"/>
+      <c r="FJ9" s="0"/>
+      <c r="FK9" s="0"/>
+      <c r="FL9" s="0"/>
+      <c r="FM9" s="0"/>
+      <c r="FN9" s="0"/>
+      <c r="FO9" s="0"/>
+      <c r="FP9" s="0"/>
+      <c r="FQ9" s="0"/>
+      <c r="FR9" s="0"/>
+      <c r="FS9" s="0"/>
+      <c r="FT9" s="0"/>
+      <c r="FU9" s="0"/>
+      <c r="FV9" s="0"/>
+      <c r="FW9" s="0"/>
+      <c r="FX9" s="0"/>
+      <c r="FY9" s="0"/>
+      <c r="FZ9" s="0"/>
+      <c r="GA9" s="0"/>
+      <c r="GB9" s="0"/>
+      <c r="GC9" s="0"/>
+      <c r="GD9" s="0"/>
+      <c r="GE9" s="0"/>
+      <c r="GF9" s="0"/>
+      <c r="GG9" s="0"/>
+      <c r="GH9" s="0"/>
+      <c r="GI9" s="0"/>
+      <c r="GJ9" s="0"/>
+      <c r="GK9" s="0"/>
+      <c r="GL9" s="0"/>
+      <c r="GM9" s="0"/>
+      <c r="GN9" s="0"/>
+      <c r="GO9" s="0"/>
+      <c r="GP9" s="0"/>
+      <c r="GQ9" s="0"/>
+      <c r="GR9" s="0"/>
+      <c r="GS9" s="0"/>
+      <c r="GT9" s="0"/>
+      <c r="GU9" s="0"/>
+      <c r="GV9" s="0"/>
+      <c r="GW9" s="0"/>
+      <c r="GX9" s="0"/>
+      <c r="GY9" s="0"/>
+      <c r="GZ9" s="0"/>
+      <c r="HA9" s="0"/>
+      <c r="HB9" s="0"/>
+      <c r="HC9" s="0"/>
+      <c r="HD9" s="0"/>
+      <c r="HE9" s="0"/>
+      <c r="HF9" s="0"/>
+      <c r="HG9" s="0"/>
+      <c r="HH9" s="0"/>
+      <c r="HI9" s="0"/>
+      <c r="HJ9" s="0"/>
+      <c r="HK9" s="0"/>
+      <c r="HL9" s="0"/>
+      <c r="HM9" s="0"/>
+      <c r="HN9" s="0"/>
+      <c r="HO9" s="0"/>
+      <c r="HP9" s="0"/>
+      <c r="HQ9" s="0"/>
+      <c r="HR9" s="0"/>
+      <c r="HS9" s="0"/>
+      <c r="HT9" s="0"/>
+      <c r="HU9" s="0"/>
+      <c r="HV9" s="0"/>
+      <c r="HW9" s="0"/>
+      <c r="HX9" s="0"/>
+      <c r="HY9" s="0"/>
+      <c r="HZ9" s="0"/>
+      <c r="IA9" s="0"/>
+      <c r="IB9" s="0"/>
+      <c r="IC9" s="0"/>
+      <c r="ID9" s="0"/>
+      <c r="IE9" s="0"/>
+      <c r="IF9" s="0"/>
+      <c r="IG9" s="0"/>
+      <c r="IH9" s="0"/>
+      <c r="II9" s="0"/>
+      <c r="IJ9" s="0"/>
+      <c r="IK9" s="0"/>
+      <c r="IL9" s="0"/>
+      <c r="IM9" s="0"/>
+      <c r="IN9" s="0"/>
+      <c r="IO9" s="0"/>
+      <c r="IP9" s="0"/>
+      <c r="IQ9" s="0"/>
+      <c r="IR9" s="0"/>
+      <c r="IS9" s="0"/>
+      <c r="IT9" s="0"/>
+      <c r="IU9" s="0"/>
+      <c r="IV9" s="0"/>
+      <c r="IW9" s="0"/>
+      <c r="IX9" s="0"/>
+      <c r="IY9" s="0"/>
+      <c r="IZ9" s="0"/>
+      <c r="JA9" s="0"/>
+      <c r="JB9" s="0"/>
+      <c r="JC9" s="0"/>
+      <c r="JD9" s="0"/>
+      <c r="JE9" s="0"/>
+      <c r="JF9" s="0"/>
+      <c r="JG9" s="0"/>
+      <c r="JH9" s="0"/>
+      <c r="JI9" s="0"/>
+      <c r="JJ9" s="0"/>
+      <c r="JK9" s="0"/>
+      <c r="JL9" s="0"/>
+      <c r="JM9" s="0"/>
+      <c r="JN9" s="0"/>
+      <c r="JO9" s="0"/>
+      <c r="JP9" s="0"/>
+      <c r="JQ9" s="0"/>
+      <c r="JR9" s="0"/>
+      <c r="JS9" s="0"/>
+      <c r="JT9" s="0"/>
+      <c r="JU9" s="0"/>
+      <c r="JV9" s="0"/>
+      <c r="JW9" s="0"/>
+      <c r="JX9" s="0"/>
+      <c r="JY9" s="0"/>
+      <c r="JZ9" s="0"/>
+      <c r="KA9" s="0"/>
+      <c r="KB9" s="0"/>
+      <c r="KC9" s="0"/>
+      <c r="KD9" s="0"/>
+      <c r="KE9" s="0"/>
+      <c r="KF9" s="0"/>
+      <c r="KG9" s="0"/>
+      <c r="KH9" s="0"/>
+      <c r="KI9" s="0"/>
+      <c r="KJ9" s="0"/>
+      <c r="KK9" s="0"/>
+      <c r="KL9" s="0"/>
+      <c r="KM9" s="0"/>
+      <c r="KN9" s="0"/>
+      <c r="KO9" s="0"/>
+      <c r="KP9" s="0"/>
+      <c r="KQ9" s="0"/>
+      <c r="KR9" s="0"/>
+      <c r="KS9" s="0"/>
+      <c r="KT9" s="0"/>
+      <c r="KU9" s="0"/>
+      <c r="KV9" s="0"/>
+      <c r="KW9" s="0"/>
+      <c r="KX9" s="0"/>
+      <c r="KY9" s="0"/>
+      <c r="KZ9" s="0"/>
+      <c r="LA9" s="0"/>
+      <c r="LB9" s="0"/>
+      <c r="LC9" s="0"/>
+      <c r="LD9" s="0"/>
+      <c r="LE9" s="0"/>
+      <c r="LF9" s="0"/>
+      <c r="LG9" s="0"/>
+      <c r="LH9" s="0"/>
+      <c r="LI9" s="0"/>
+      <c r="LJ9" s="0"/>
+      <c r="LK9" s="0"/>
+      <c r="LL9" s="0"/>
+      <c r="LM9" s="0"/>
+      <c r="LN9" s="0"/>
+      <c r="LO9" s="0"/>
+      <c r="LP9" s="0"/>
+      <c r="LQ9" s="0"/>
+      <c r="LR9" s="0"/>
+      <c r="LS9" s="0"/>
+      <c r="LT9" s="0"/>
+      <c r="LU9" s="0"/>
+      <c r="LV9" s="0"/>
+      <c r="LW9" s="0"/>
+      <c r="LX9" s="0"/>
+      <c r="LY9" s="0"/>
+      <c r="LZ9" s="0"/>
+      <c r="MA9" s="0"/>
+      <c r="MB9" s="0"/>
+      <c r="MC9" s="0"/>
+      <c r="MD9" s="0"/>
+      <c r="ME9" s="0"/>
+      <c r="MF9" s="0"/>
+      <c r="MG9" s="0"/>
+      <c r="MH9" s="0"/>
+      <c r="MI9" s="0"/>
+      <c r="MJ9" s="0"/>
+      <c r="MK9" s="0"/>
+      <c r="ML9" s="0"/>
+      <c r="MM9" s="0"/>
+      <c r="MN9" s="0"/>
+      <c r="MO9" s="0"/>
+      <c r="MP9" s="0"/>
+      <c r="MQ9" s="0"/>
+      <c r="MR9" s="0"/>
+      <c r="MS9" s="0"/>
+      <c r="MT9" s="0"/>
+      <c r="MU9" s="0"/>
+      <c r="MV9" s="0"/>
+      <c r="MW9" s="0"/>
+      <c r="MX9" s="0"/>
+      <c r="MY9" s="0"/>
+      <c r="MZ9" s="0"/>
+      <c r="NA9" s="0"/>
+      <c r="NB9" s="0"/>
+      <c r="NC9" s="0"/>
+      <c r="ND9" s="0"/>
+      <c r="NE9" s="0"/>
+      <c r="NF9" s="0"/>
+      <c r="NG9" s="0"/>
+      <c r="NH9" s="0"/>
+      <c r="NI9" s="0"/>
+      <c r="NJ9" s="0"/>
+      <c r="NK9" s="0"/>
+      <c r="NL9" s="0"/>
+      <c r="NM9" s="0"/>
+      <c r="NN9" s="0"/>
+      <c r="NO9" s="0"/>
+      <c r="NP9" s="0"/>
+      <c r="NQ9" s="0"/>
+      <c r="NR9" s="0"/>
+      <c r="NS9" s="0"/>
+      <c r="NT9" s="0"/>
+      <c r="NU9" s="0"/>
+      <c r="NV9" s="0"/>
+      <c r="NW9" s="0"/>
+      <c r="NX9" s="0"/>
+      <c r="NY9" s="0"/>
+      <c r="NZ9" s="0"/>
+      <c r="OA9" s="0"/>
+      <c r="OB9" s="0"/>
+      <c r="OC9" s="0"/>
+      <c r="OD9" s="0"/>
+      <c r="OE9" s="0"/>
+      <c r="OF9" s="0"/>
+      <c r="OG9" s="0"/>
+      <c r="OH9" s="0"/>
+      <c r="OI9" s="0"/>
+      <c r="OJ9" s="0"/>
+      <c r="OK9" s="0"/>
+      <c r="OL9" s="0"/>
+      <c r="OM9" s="0"/>
+      <c r="ON9" s="0"/>
+      <c r="OO9" s="0"/>
+      <c r="OP9" s="0"/>
+      <c r="OQ9" s="0"/>
+      <c r="OR9" s="0"/>
+      <c r="OS9" s="0"/>
+      <c r="OT9" s="0"/>
+      <c r="OU9" s="0"/>
+      <c r="OV9" s="0"/>
+      <c r="OW9" s="0"/>
+      <c r="OX9" s="0"/>
+      <c r="OY9" s="0"/>
+      <c r="OZ9" s="0"/>
+      <c r="PA9" s="0"/>
+      <c r="PB9" s="0"/>
+      <c r="PC9" s="0"/>
+      <c r="PD9" s="0"/>
+      <c r="PE9" s="0"/>
+      <c r="PF9" s="0"/>
+      <c r="PG9" s="0"/>
+      <c r="PH9" s="0"/>
+      <c r="PI9" s="0"/>
+      <c r="PJ9" s="0"/>
+      <c r="PK9" s="0"/>
+      <c r="PL9" s="0"/>
+      <c r="PM9" s="0"/>
+      <c r="PN9" s="0"/>
+      <c r="PO9" s="0"/>
+      <c r="PP9" s="0"/>
+      <c r="PQ9" s="0"/>
+      <c r="PR9" s="0"/>
+      <c r="PS9" s="0"/>
+      <c r="PT9" s="0"/>
+      <c r="PU9" s="0"/>
+      <c r="PV9" s="0"/>
+      <c r="PW9" s="0"/>
+      <c r="PX9" s="0"/>
+      <c r="PY9" s="0"/>
+      <c r="PZ9" s="0"/>
+      <c r="QA9" s="0"/>
+      <c r="QB9" s="0"/>
+      <c r="QC9" s="0"/>
+      <c r="QD9" s="0"/>
+      <c r="QE9" s="0"/>
+      <c r="QF9" s="0"/>
+      <c r="QG9" s="0"/>
+      <c r="QH9" s="0"/>
+      <c r="QI9" s="0"/>
+      <c r="QJ9" s="0"/>
+      <c r="QK9" s="0"/>
+      <c r="QL9" s="0"/>
+      <c r="QM9" s="0"/>
+      <c r="QN9" s="0"/>
+      <c r="QO9" s="0"/>
+      <c r="QP9" s="0"/>
+      <c r="QQ9" s="0"/>
+      <c r="QR9" s="0"/>
+      <c r="QS9" s="0"/>
+      <c r="QT9" s="0"/>
+      <c r="QU9" s="0"/>
+      <c r="QV9" s="0"/>
+      <c r="QW9" s="0"/>
+      <c r="QX9" s="0"/>
+      <c r="QY9" s="0"/>
+      <c r="QZ9" s="0"/>
+      <c r="RA9" s="0"/>
+      <c r="RB9" s="0"/>
+      <c r="RC9" s="0"/>
+      <c r="RD9" s="0"/>
+      <c r="RE9" s="0"/>
+      <c r="RF9" s="0"/>
+      <c r="RG9" s="0"/>
+      <c r="RH9" s="0"/>
+      <c r="RI9" s="0"/>
+      <c r="RJ9" s="0"/>
+      <c r="RK9" s="0"/>
+      <c r="RL9" s="0"/>
+      <c r="RM9" s="0"/>
+      <c r="RN9" s="0"/>
+      <c r="RO9" s="0"/>
+      <c r="RP9" s="0"/>
+      <c r="RQ9" s="0"/>
+      <c r="RR9" s="0"/>
+      <c r="RS9" s="0"/>
+      <c r="RT9" s="0"/>
+      <c r="RU9" s="0"/>
+      <c r="RV9" s="0"/>
+      <c r="RW9" s="0"/>
+      <c r="RX9" s="0"/>
+      <c r="RY9" s="0"/>
+      <c r="RZ9" s="0"/>
+      <c r="SA9" s="0"/>
+      <c r="SB9" s="0"/>
+      <c r="SC9" s="0"/>
+      <c r="SD9" s="0"/>
+      <c r="SE9" s="0"/>
+      <c r="SF9" s="0"/>
+      <c r="SG9" s="0"/>
+      <c r="SH9" s="0"/>
+      <c r="SI9" s="0"/>
+      <c r="SJ9" s="0"/>
+      <c r="SK9" s="0"/>
+      <c r="SL9" s="0"/>
+      <c r="SM9" s="0"/>
+      <c r="SN9" s="0"/>
+      <c r="SO9" s="0"/>
+      <c r="SP9" s="0"/>
+      <c r="SQ9" s="0"/>
+      <c r="SR9" s="0"/>
+      <c r="SS9" s="0"/>
+      <c r="ST9" s="0"/>
+      <c r="SU9" s="0"/>
+      <c r="SV9" s="0"/>
+      <c r="SW9" s="0"/>
+      <c r="SX9" s="0"/>
+      <c r="SY9" s="0"/>
+      <c r="SZ9" s="0"/>
+      <c r="TA9" s="0"/>
+      <c r="TB9" s="0"/>
+      <c r="TC9" s="0"/>
+      <c r="TD9" s="0"/>
+      <c r="TE9" s="0"/>
+      <c r="TF9" s="0"/>
+      <c r="TG9" s="0"/>
+      <c r="TH9" s="0"/>
+      <c r="TI9" s="0"/>
+      <c r="TJ9" s="0"/>
+      <c r="TK9" s="0"/>
+      <c r="TL9" s="0"/>
+      <c r="TM9" s="0"/>
+      <c r="TN9" s="0"/>
+      <c r="TO9" s="0"/>
+      <c r="TP9" s="0"/>
+      <c r="TQ9" s="0"/>
+      <c r="TR9" s="0"/>
+      <c r="TS9" s="0"/>
+      <c r="TT9" s="0"/>
+      <c r="TU9" s="0"/>
+      <c r="TV9" s="0"/>
+      <c r="TW9" s="0"/>
+      <c r="TX9" s="0"/>
+      <c r="TY9" s="0"/>
+      <c r="TZ9" s="0"/>
+      <c r="UA9" s="0"/>
+      <c r="UB9" s="0"/>
+      <c r="UC9" s="0"/>
+      <c r="UD9" s="0"/>
+      <c r="UE9" s="0"/>
+      <c r="UF9" s="0"/>
+      <c r="UG9" s="0"/>
+      <c r="UH9" s="0"/>
+      <c r="UI9" s="0"/>
+      <c r="UJ9" s="0"/>
+      <c r="UK9" s="0"/>
+      <c r="UL9" s="0"/>
+      <c r="UM9" s="0"/>
+      <c r="UN9" s="0"/>
+      <c r="UO9" s="0"/>
+      <c r="UP9" s="0"/>
+      <c r="UQ9" s="0"/>
+      <c r="UR9" s="0"/>
+      <c r="US9" s="0"/>
+      <c r="UT9" s="0"/>
+      <c r="UU9" s="0"/>
+      <c r="UV9" s="0"/>
+      <c r="UW9" s="0"/>
+      <c r="UX9" s="0"/>
+      <c r="UY9" s="0"/>
+      <c r="UZ9" s="0"/>
+      <c r="VA9" s="0"/>
+      <c r="VB9" s="0"/>
+      <c r="VC9" s="0"/>
+      <c r="VD9" s="0"/>
+      <c r="VE9" s="0"/>
+      <c r="VF9" s="0"/>
+      <c r="VG9" s="0"/>
+      <c r="VH9" s="0"/>
+      <c r="VI9" s="0"/>
+      <c r="VJ9" s="0"/>
+      <c r="VK9" s="0"/>
+      <c r="VL9" s="0"/>
+      <c r="VM9" s="0"/>
+      <c r="VN9" s="0"/>
+      <c r="VO9" s="0"/>
+      <c r="VP9" s="0"/>
+      <c r="VQ9" s="0"/>
+      <c r="VR9" s="0"/>
+      <c r="VS9" s="0"/>
+      <c r="VT9" s="0"/>
+      <c r="VU9" s="0"/>
+      <c r="VV9" s="0"/>
+      <c r="VW9" s="0"/>
+      <c r="VX9" s="0"/>
+      <c r="VY9" s="0"/>
+      <c r="VZ9" s="0"/>
+      <c r="WA9" s="0"/>
+      <c r="WB9" s="0"/>
+      <c r="WC9" s="0"/>
+      <c r="WD9" s="0"/>
+      <c r="WE9" s="0"/>
+      <c r="WF9" s="0"/>
+      <c r="WG9" s="0"/>
+      <c r="WH9" s="0"/>
+      <c r="WI9" s="0"/>
+      <c r="WJ9" s="0"/>
+      <c r="WK9" s="0"/>
+      <c r="WL9" s="0"/>
+      <c r="WM9" s="0"/>
+      <c r="WN9" s="0"/>
+      <c r="WO9" s="0"/>
+      <c r="WP9" s="0"/>
+      <c r="WQ9" s="0"/>
+      <c r="WR9" s="0"/>
+      <c r="WS9" s="0"/>
+      <c r="WT9" s="0"/>
+      <c r="WU9" s="0"/>
+      <c r="WV9" s="0"/>
+      <c r="WW9" s="0"/>
+      <c r="WX9" s="0"/>
+      <c r="WY9" s="0"/>
+      <c r="WZ9" s="0"/>
+      <c r="XA9" s="0"/>
+      <c r="XB9" s="0"/>
+      <c r="XC9" s="0"/>
+      <c r="XD9" s="0"/>
+      <c r="XE9" s="0"/>
+      <c r="XF9" s="0"/>
+      <c r="XG9" s="0"/>
+      <c r="XH9" s="0"/>
+      <c r="XI9" s="0"/>
+      <c r="XJ9" s="0"/>
+      <c r="XK9" s="0"/>
+      <c r="XL9" s="0"/>
+      <c r="XM9" s="0"/>
+      <c r="XN9" s="0"/>
+      <c r="XO9" s="0"/>
+      <c r="XP9" s="0"/>
+      <c r="XQ9" s="0"/>
+      <c r="XR9" s="0"/>
+      <c r="XS9" s="0"/>
+      <c r="XT9" s="0"/>
+      <c r="XU9" s="0"/>
+      <c r="XV9" s="0"/>
+      <c r="XW9" s="0"/>
+      <c r="XX9" s="0"/>
+      <c r="XY9" s="0"/>
+      <c r="XZ9" s="0"/>
+      <c r="YA9" s="0"/>
+      <c r="YB9" s="0"/>
+      <c r="YC9" s="0"/>
+      <c r="YD9" s="0"/>
+      <c r="YE9" s="0"/>
+      <c r="YF9" s="0"/>
+      <c r="YG9" s="0"/>
+      <c r="YH9" s="0"/>
+      <c r="YI9" s="0"/>
+      <c r="YJ9" s="0"/>
+      <c r="YK9" s="0"/>
+      <c r="YL9" s="0"/>
+      <c r="YM9" s="0"/>
+      <c r="YN9" s="0"/>
+      <c r="YO9" s="0"/>
+      <c r="YP9" s="0"/>
+      <c r="YQ9" s="0"/>
+      <c r="YR9" s="0"/>
+      <c r="YS9" s="0"/>
+      <c r="YT9" s="0"/>
+      <c r="YU9" s="0"/>
+      <c r="YV9" s="0"/>
+      <c r="YW9" s="0"/>
+      <c r="YX9" s="0"/>
+      <c r="YY9" s="0"/>
+      <c r="YZ9" s="0"/>
+      <c r="ZA9" s="0"/>
+      <c r="ZB9" s="0"/>
+      <c r="ZC9" s="0"/>
+      <c r="ZD9" s="0"/>
+      <c r="ZE9" s="0"/>
+      <c r="ZF9" s="0"/>
+      <c r="ZG9" s="0"/>
+      <c r="ZH9" s="0"/>
+      <c r="ZI9" s="0"/>
+      <c r="ZJ9" s="0"/>
+      <c r="ZK9" s="0"/>
+      <c r="ZL9" s="0"/>
+      <c r="ZM9" s="0"/>
+      <c r="ZN9" s="0"/>
+      <c r="ZO9" s="0"/>
+      <c r="ZP9" s="0"/>
+      <c r="ZQ9" s="0"/>
+      <c r="ZR9" s="0"/>
+      <c r="ZS9" s="0"/>
+      <c r="ZT9" s="0"/>
+      <c r="ZU9" s="0"/>
+      <c r="ZV9" s="0"/>
+      <c r="ZW9" s="0"/>
+      <c r="ZX9" s="0"/>
+      <c r="ZY9" s="0"/>
+      <c r="ZZ9" s="0"/>
+      <c r="AAA9" s="0"/>
+      <c r="AAB9" s="0"/>
+      <c r="AAC9" s="0"/>
+      <c r="AAD9" s="0"/>
+      <c r="AAE9" s="0"/>
+      <c r="AAF9" s="0"/>
+      <c r="AAG9" s="0"/>
+      <c r="AAH9" s="0"/>
+      <c r="AAI9" s="0"/>
+      <c r="AAJ9" s="0"/>
+      <c r="AAK9" s="0"/>
+      <c r="AAL9" s="0"/>
+      <c r="AAM9" s="0"/>
+      <c r="AAN9" s="0"/>
+      <c r="AAO9" s="0"/>
+      <c r="AAP9" s="0"/>
+      <c r="AAQ9" s="0"/>
+      <c r="AAR9" s="0"/>
+      <c r="AAS9" s="0"/>
+      <c r="AAT9" s="0"/>
+      <c r="AAU9" s="0"/>
+      <c r="AAV9" s="0"/>
+      <c r="AAW9" s="0"/>
+      <c r="AAX9" s="0"/>
+      <c r="AAY9" s="0"/>
+      <c r="AAZ9" s="0"/>
+      <c r="ABA9" s="0"/>
+      <c r="ABB9" s="0"/>
+      <c r="ABC9" s="0"/>
+      <c r="ABD9" s="0"/>
+      <c r="ABE9" s="0"/>
+      <c r="ABF9" s="0"/>
+      <c r="ABG9" s="0"/>
+      <c r="ABH9" s="0"/>
+      <c r="ABI9" s="0"/>
+      <c r="ABJ9" s="0"/>
+      <c r="ABK9" s="0"/>
+      <c r="ABL9" s="0"/>
+      <c r="ABM9" s="0"/>
+      <c r="ABN9" s="0"/>
+      <c r="ABO9" s="0"/>
+      <c r="ABP9" s="0"/>
+      <c r="ABQ9" s="0"/>
+      <c r="ABR9" s="0"/>
+      <c r="ABS9" s="0"/>
+      <c r="ABT9" s="0"/>
+      <c r="ABU9" s="0"/>
+      <c r="ABV9" s="0"/>
+      <c r="ABW9" s="0"/>
+      <c r="ABX9" s="0"/>
+      <c r="ABY9" s="0"/>
+      <c r="ABZ9" s="0"/>
+      <c r="ACA9" s="0"/>
+      <c r="ACB9" s="0"/>
+      <c r="ACC9" s="0"/>
+      <c r="ACD9" s="0"/>
+      <c r="ACE9" s="0"/>
+      <c r="ACF9" s="0"/>
+      <c r="ACG9" s="0"/>
+      <c r="ACH9" s="0"/>
+      <c r="ACI9" s="0"/>
+      <c r="ACJ9" s="0"/>
+      <c r="ACK9" s="0"/>
+      <c r="ACL9" s="0"/>
+      <c r="ACM9" s="0"/>
+      <c r="ACN9" s="0"/>
+      <c r="ACO9" s="0"/>
+      <c r="ACP9" s="0"/>
+      <c r="ACQ9" s="0"/>
+      <c r="ACR9" s="0"/>
+      <c r="ACS9" s="0"/>
+      <c r="ACT9" s="0"/>
+      <c r="ACU9" s="0"/>
+      <c r="ACV9" s="0"/>
+      <c r="ACW9" s="0"/>
+      <c r="ACX9" s="0"/>
+      <c r="ACY9" s="0"/>
+      <c r="ACZ9" s="0"/>
+      <c r="ADA9" s="0"/>
+      <c r="ADB9" s="0"/>
+      <c r="ADC9" s="0"/>
+      <c r="ADD9" s="0"/>
+      <c r="ADE9" s="0"/>
+      <c r="ADF9" s="0"/>
+      <c r="ADG9" s="0"/>
+      <c r="ADH9" s="0"/>
+      <c r="ADI9" s="0"/>
+      <c r="ADJ9" s="0"/>
+      <c r="ADK9" s="0"/>
+      <c r="ADL9" s="0"/>
+      <c r="ADM9" s="0"/>
+      <c r="ADN9" s="0"/>
+      <c r="ADO9" s="0"/>
+      <c r="ADP9" s="0"/>
+      <c r="ADQ9" s="0"/>
+      <c r="ADR9" s="0"/>
+      <c r="ADS9" s="0"/>
+      <c r="ADT9" s="0"/>
+      <c r="ADU9" s="0"/>
+      <c r="ADV9" s="0"/>
+      <c r="ADW9" s="0"/>
+      <c r="ADX9" s="0"/>
+      <c r="ADY9" s="0"/>
+      <c r="ADZ9" s="0"/>
+      <c r="AEA9" s="0"/>
+      <c r="AEB9" s="0"/>
+      <c r="AEC9" s="0"/>
+      <c r="AED9" s="0"/>
+      <c r="AEE9" s="0"/>
+      <c r="AEF9" s="0"/>
+      <c r="AEG9" s="0"/>
+      <c r="AEH9" s="0"/>
+      <c r="AEI9" s="0"/>
+      <c r="AEJ9" s="0"/>
+      <c r="AEK9" s="0"/>
+      <c r="AEL9" s="0"/>
+      <c r="AEM9" s="0"/>
+      <c r="AEN9" s="0"/>
+      <c r="AEO9" s="0"/>
+      <c r="AEP9" s="0"/>
+      <c r="AEQ9" s="0"/>
+      <c r="AER9" s="0"/>
+      <c r="AES9" s="0"/>
+      <c r="AET9" s="0"/>
+      <c r="AEU9" s="0"/>
+      <c r="AEV9" s="0"/>
+      <c r="AEW9" s="0"/>
+      <c r="AEX9" s="0"/>
+      <c r="AEY9" s="0"/>
+      <c r="AEZ9" s="0"/>
+      <c r="AFA9" s="0"/>
+      <c r="AFB9" s="0"/>
+      <c r="AFC9" s="0"/>
+      <c r="AFD9" s="0"/>
+      <c r="AFE9" s="0"/>
+      <c r="AFF9" s="0"/>
+      <c r="AFG9" s="0"/>
+      <c r="AFH9" s="0"/>
+      <c r="AFI9" s="0"/>
+      <c r="AFJ9" s="0"/>
+      <c r="AFK9" s="0"/>
+      <c r="AFL9" s="0"/>
+      <c r="AFM9" s="0"/>
+      <c r="AFN9" s="0"/>
+      <c r="AFO9" s="0"/>
+      <c r="AFP9" s="0"/>
+      <c r="AFQ9" s="0"/>
+      <c r="AFR9" s="0"/>
+      <c r="AFS9" s="0"/>
+      <c r="AFT9" s="0"/>
+      <c r="AFU9" s="0"/>
+      <c r="AFV9" s="0"/>
+      <c r="AFW9" s="0"/>
+      <c r="AFX9" s="0"/>
+      <c r="AFY9" s="0"/>
+      <c r="AFZ9" s="0"/>
+      <c r="AGA9" s="0"/>
+      <c r="AGB9" s="0"/>
+      <c r="AGC9" s="0"/>
+      <c r="AGD9" s="0"/>
+      <c r="AGE9" s="0"/>
+      <c r="AGF9" s="0"/>
+      <c r="AGG9" s="0"/>
+      <c r="AGH9" s="0"/>
+      <c r="AGI9" s="0"/>
+      <c r="AGJ9" s="0"/>
+      <c r="AGK9" s="0"/>
+      <c r="AGL9" s="0"/>
+      <c r="AGM9" s="0"/>
+      <c r="AGN9" s="0"/>
+      <c r="AGO9" s="0"/>
+      <c r="AGP9" s="0"/>
+      <c r="AGQ9" s="0"/>
+      <c r="AGR9" s="0"/>
+      <c r="AGS9" s="0"/>
+      <c r="AGT9" s="0"/>
+      <c r="AGU9" s="0"/>
+      <c r="AGV9" s="0"/>
+      <c r="AGW9" s="0"/>
+      <c r="AGX9" s="0"/>
+      <c r="AGY9" s="0"/>
+      <c r="AGZ9" s="0"/>
+      <c r="AHA9" s="0"/>
+      <c r="AHB9" s="0"/>
+      <c r="AHC9" s="0"/>
+      <c r="AHD9" s="0"/>
+      <c r="AHE9" s="0"/>
+      <c r="AHF9" s="0"/>
+      <c r="AHG9" s="0"/>
+      <c r="AHH9" s="0"/>
+      <c r="AHI9" s="0"/>
+      <c r="AHJ9" s="0"/>
+      <c r="AHK9" s="0"/>
+      <c r="AHL9" s="0"/>
+      <c r="AHM9" s="0"/>
+      <c r="AHN9" s="0"/>
+      <c r="AHO9" s="0"/>
+      <c r="AHP9" s="0"/>
+      <c r="AHQ9" s="0"/>
+      <c r="AHR9" s="0"/>
+      <c r="AHS9" s="0"/>
+      <c r="AHT9" s="0"/>
+      <c r="AHU9" s="0"/>
+      <c r="AHV9" s="0"/>
+      <c r="AHW9" s="0"/>
+      <c r="AHX9" s="0"/>
+      <c r="AHY9" s="0"/>
+      <c r="AHZ9" s="0"/>
+      <c r="AIA9" s="0"/>
+      <c r="AIB9" s="0"/>
+      <c r="AIC9" s="0"/>
+      <c r="AID9" s="0"/>
+      <c r="AIE9" s="0"/>
+      <c r="AIF9" s="0"/>
+      <c r="AIG9" s="0"/>
+      <c r="AIH9" s="0"/>
+      <c r="AII9" s="0"/>
+      <c r="AIJ9" s="0"/>
+      <c r="AIK9" s="0"/>
+      <c r="AIL9" s="0"/>
+      <c r="AIM9" s="0"/>
+      <c r="AIN9" s="0"/>
+      <c r="AIO9" s="0"/>
+      <c r="AIP9" s="0"/>
+      <c r="AIQ9" s="0"/>
+      <c r="AIR9" s="0"/>
+      <c r="AIS9" s="0"/>
+      <c r="AIT9" s="0"/>
+      <c r="AIU9" s="0"/>
+      <c r="AIV9" s="0"/>
+      <c r="AIW9" s="0"/>
+      <c r="AIX9" s="0"/>
+      <c r="AIY9" s="0"/>
+      <c r="AIZ9" s="0"/>
+      <c r="AJA9" s="0"/>
+      <c r="AJB9" s="0"/>
+      <c r="AJC9" s="0"/>
+      <c r="AJD9" s="0"/>
+      <c r="AJE9" s="0"/>
+      <c r="AJF9" s="0"/>
+      <c r="AJG9" s="0"/>
+      <c r="AJH9" s="0"/>
+      <c r="AJI9" s="0"/>
+      <c r="AJJ9" s="0"/>
+      <c r="AJK9" s="0"/>
+      <c r="AJL9" s="0"/>
+      <c r="AJM9" s="0"/>
+      <c r="AJN9" s="0"/>
+      <c r="AJO9" s="0"/>
+      <c r="AJP9" s="0"/>
+      <c r="AJQ9" s="0"/>
+      <c r="AJR9" s="0"/>
+      <c r="AJS9" s="0"/>
+      <c r="AJT9" s="0"/>
+      <c r="AJU9" s="0"/>
+      <c r="AJV9" s="0"/>
+      <c r="AJW9" s="0"/>
+      <c r="AJX9" s="0"/>
+      <c r="AJY9" s="0"/>
+      <c r="AJZ9" s="0"/>
+      <c r="AKA9" s="0"/>
+      <c r="AKB9" s="0"/>
+      <c r="AKC9" s="0"/>
+      <c r="AKD9" s="0"/>
+      <c r="AKE9" s="0"/>
+      <c r="AKF9" s="0"/>
+      <c r="AKG9" s="0"/>
+      <c r="AKH9" s="0"/>
+      <c r="AKI9" s="0"/>
+      <c r="AKJ9" s="0"/>
+      <c r="AKK9" s="0"/>
+      <c r="AKL9" s="0"/>
+      <c r="AKM9" s="0"/>
+      <c r="AKN9" s="0"/>
+      <c r="AKO9" s="0"/>
+      <c r="AKP9" s="0"/>
+      <c r="AKQ9" s="0"/>
+      <c r="AKR9" s="0"/>
+      <c r="AKS9" s="0"/>
+      <c r="AKT9" s="0"/>
+      <c r="AKU9" s="0"/>
+      <c r="AKV9" s="0"/>
+      <c r="AKW9" s="0"/>
+      <c r="AKX9" s="0"/>
+      <c r="AKY9" s="0"/>
+      <c r="AKZ9" s="0"/>
+      <c r="ALA9" s="0"/>
+      <c r="ALB9" s="0"/>
+      <c r="ALC9" s="0"/>
+      <c r="ALD9" s="0"/>
+      <c r="ALE9" s="0"/>
+      <c r="ALF9" s="0"/>
+      <c r="ALG9" s="0"/>
+      <c r="ALH9" s="0"/>
+      <c r="ALI9" s="0"/>
+      <c r="ALJ9" s="0"/>
+      <c r="ALK9" s="0"/>
+      <c r="ALL9" s="0"/>
+      <c r="ALM9" s="0"/>
+      <c r="ALN9" s="0"/>
+      <c r="ALO9" s="0"/>
+      <c r="ALP9" s="0"/>
+      <c r="ALQ9" s="0"/>
+      <c r="ALR9" s="0"/>
+      <c r="ALS9" s="0"/>
+      <c r="ALT9" s="0"/>
+      <c r="ALU9" s="0"/>
+      <c r="ALV9" s="0"/>
+      <c r="ALW9" s="0"/>
+      <c r="ALX9" s="0"/>
+      <c r="ALY9" s="0"/>
+      <c r="ALZ9" s="0"/>
+      <c r="AMA9" s="0"/>
+      <c r="AMB9" s="0"/>
+      <c r="AMC9" s="0"/>
+      <c r="AMD9" s="0"/>
+      <c r="AME9" s="0"/>
+      <c r="AMF9" s="0"/>
+      <c r="AMG9" s="0"/>
+      <c r="AMH9" s="0"/>
+      <c r="AMI9" s="0"/>
+      <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>27</v>
@@ -9270,128 +10311,1243 @@
         <v>0</v>
       </c>
       <c r="K10" s="7"/>
-      <c r="AMJ10" s="10"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="0"/>
+      <c r="O10" s="0"/>
+      <c r="P10" s="0"/>
+      <c r="Q10" s="0"/>
+      <c r="R10" s="0"/>
+      <c r="S10" s="0"/>
+      <c r="T10" s="0"/>
+      <c r="U10" s="0"/>
+      <c r="V10" s="0"/>
+      <c r="W10" s="0"/>
+      <c r="X10" s="0"/>
+      <c r="Y10" s="0"/>
+      <c r="Z10" s="0"/>
+      <c r="AA10" s="0"/>
+      <c r="AB10" s="0"/>
+      <c r="AC10" s="0"/>
+      <c r="AD10" s="0"/>
+      <c r="AE10" s="0"/>
+      <c r="AF10" s="0"/>
+      <c r="AG10" s="0"/>
+      <c r="AH10" s="0"/>
+      <c r="AI10" s="0"/>
+      <c r="AJ10" s="0"/>
+      <c r="AK10" s="0"/>
+      <c r="AL10" s="0"/>
+      <c r="AM10" s="0"/>
+      <c r="AN10" s="0"/>
+      <c r="AO10" s="0"/>
+      <c r="AP10" s="0"/>
+      <c r="AQ10" s="0"/>
+      <c r="AR10" s="0"/>
+      <c r="AS10" s="0"/>
+      <c r="AT10" s="0"/>
+      <c r="AU10" s="0"/>
+      <c r="AV10" s="0"/>
+      <c r="AW10" s="0"/>
+      <c r="AX10" s="0"/>
+      <c r="AY10" s="0"/>
+      <c r="AZ10" s="0"/>
+      <c r="BA10" s="0"/>
+      <c r="BB10" s="0"/>
+      <c r="BC10" s="0"/>
+      <c r="BD10" s="0"/>
+      <c r="BE10" s="0"/>
+      <c r="BF10" s="0"/>
+      <c r="BG10" s="0"/>
+      <c r="BH10" s="0"/>
+      <c r="BI10" s="0"/>
+      <c r="BJ10" s="0"/>
+      <c r="BK10" s="0"/>
+      <c r="BL10" s="0"/>
+      <c r="BM10" s="0"/>
+      <c r="BN10" s="0"/>
+      <c r="BO10" s="0"/>
+      <c r="BP10" s="0"/>
+      <c r="BQ10" s="0"/>
+      <c r="BR10" s="0"/>
+      <c r="BS10" s="0"/>
+      <c r="BT10" s="0"/>
+      <c r="BU10" s="0"/>
+      <c r="BV10" s="0"/>
+      <c r="BW10" s="0"/>
+      <c r="BX10" s="0"/>
+      <c r="BY10" s="0"/>
+      <c r="BZ10" s="0"/>
+      <c r="CA10" s="0"/>
+      <c r="CB10" s="0"/>
+      <c r="CC10" s="0"/>
+      <c r="CD10" s="0"/>
+      <c r="CE10" s="0"/>
+      <c r="CF10" s="0"/>
+      <c r="CG10" s="0"/>
+      <c r="CH10" s="0"/>
+      <c r="CI10" s="0"/>
+      <c r="CJ10" s="0"/>
+      <c r="CK10" s="0"/>
+      <c r="CL10" s="0"/>
+      <c r="CM10" s="0"/>
+      <c r="CN10" s="0"/>
+      <c r="CO10" s="0"/>
+      <c r="CP10" s="0"/>
+      <c r="CQ10" s="0"/>
+      <c r="CR10" s="0"/>
+      <c r="CS10" s="0"/>
+      <c r="CT10" s="0"/>
+      <c r="CU10" s="0"/>
+      <c r="CV10" s="0"/>
+      <c r="CW10" s="0"/>
+      <c r="CX10" s="0"/>
+      <c r="CY10" s="0"/>
+      <c r="CZ10" s="0"/>
+      <c r="DA10" s="0"/>
+      <c r="DB10" s="0"/>
+      <c r="DC10" s="0"/>
+      <c r="DD10" s="0"/>
+      <c r="DE10" s="0"/>
+      <c r="DF10" s="0"/>
+      <c r="DG10" s="0"/>
+      <c r="DH10" s="0"/>
+      <c r="DI10" s="0"/>
+      <c r="DJ10" s="0"/>
+      <c r="DK10" s="0"/>
+      <c r="DL10" s="0"/>
+      <c r="DM10" s="0"/>
+      <c r="DN10" s="0"/>
+      <c r="DO10" s="0"/>
+      <c r="DP10" s="0"/>
+      <c r="DQ10" s="0"/>
+      <c r="DR10" s="0"/>
+      <c r="DS10" s="0"/>
+      <c r="DT10" s="0"/>
+      <c r="DU10" s="0"/>
+      <c r="DV10" s="0"/>
+      <c r="DW10" s="0"/>
+      <c r="DX10" s="0"/>
+      <c r="DY10" s="0"/>
+      <c r="DZ10" s="0"/>
+      <c r="EA10" s="0"/>
+      <c r="EB10" s="0"/>
+      <c r="EC10" s="0"/>
+      <c r="ED10" s="0"/>
+      <c r="EE10" s="0"/>
+      <c r="EF10" s="0"/>
+      <c r="EG10" s="0"/>
+      <c r="EH10" s="0"/>
+      <c r="EI10" s="0"/>
+      <c r="EJ10" s="0"/>
+      <c r="EK10" s="0"/>
+      <c r="EL10" s="0"/>
+      <c r="EM10" s="0"/>
+      <c r="EN10" s="0"/>
+      <c r="EO10" s="0"/>
+      <c r="EP10" s="0"/>
+      <c r="EQ10" s="0"/>
+      <c r="ER10" s="0"/>
+      <c r="ES10" s="0"/>
+      <c r="ET10" s="0"/>
+      <c r="EU10" s="0"/>
+      <c r="EV10" s="0"/>
+      <c r="EW10" s="0"/>
+      <c r="EX10" s="0"/>
+      <c r="EY10" s="0"/>
+      <c r="EZ10" s="0"/>
+      <c r="FA10" s="0"/>
+      <c r="FB10" s="0"/>
+      <c r="FC10" s="0"/>
+      <c r="FD10" s="0"/>
+      <c r="FE10" s="0"/>
+      <c r="FF10" s="0"/>
+      <c r="FG10" s="0"/>
+      <c r="FH10" s="0"/>
+      <c r="FI10" s="0"/>
+      <c r="FJ10" s="0"/>
+      <c r="FK10" s="0"/>
+      <c r="FL10" s="0"/>
+      <c r="FM10" s="0"/>
+      <c r="FN10" s="0"/>
+      <c r="FO10" s="0"/>
+      <c r="FP10" s="0"/>
+      <c r="FQ10" s="0"/>
+      <c r="FR10" s="0"/>
+      <c r="FS10" s="0"/>
+      <c r="FT10" s="0"/>
+      <c r="FU10" s="0"/>
+      <c r="FV10" s="0"/>
+      <c r="FW10" s="0"/>
+      <c r="FX10" s="0"/>
+      <c r="FY10" s="0"/>
+      <c r="FZ10" s="0"/>
+      <c r="GA10" s="0"/>
+      <c r="GB10" s="0"/>
+      <c r="GC10" s="0"/>
+      <c r="GD10" s="0"/>
+      <c r="GE10" s="0"/>
+      <c r="GF10" s="0"/>
+      <c r="GG10" s="0"/>
+      <c r="GH10" s="0"/>
+      <c r="GI10" s="0"/>
+      <c r="GJ10" s="0"/>
+      <c r="GK10" s="0"/>
+      <c r="GL10" s="0"/>
+      <c r="GM10" s="0"/>
+      <c r="GN10" s="0"/>
+      <c r="GO10" s="0"/>
+      <c r="GP10" s="0"/>
+      <c r="GQ10" s="0"/>
+      <c r="GR10" s="0"/>
+      <c r="GS10" s="0"/>
+      <c r="GT10" s="0"/>
+      <c r="GU10" s="0"/>
+      <c r="GV10" s="0"/>
+      <c r="GW10" s="0"/>
+      <c r="GX10" s="0"/>
+      <c r="GY10" s="0"/>
+      <c r="GZ10" s="0"/>
+      <c r="HA10" s="0"/>
+      <c r="HB10" s="0"/>
+      <c r="HC10" s="0"/>
+      <c r="HD10" s="0"/>
+      <c r="HE10" s="0"/>
+      <c r="HF10" s="0"/>
+      <c r="HG10" s="0"/>
+      <c r="HH10" s="0"/>
+      <c r="HI10" s="0"/>
+      <c r="HJ10" s="0"/>
+      <c r="HK10" s="0"/>
+      <c r="HL10" s="0"/>
+      <c r="HM10" s="0"/>
+      <c r="HN10" s="0"/>
+      <c r="HO10" s="0"/>
+      <c r="HP10" s="0"/>
+      <c r="HQ10" s="0"/>
+      <c r="HR10" s="0"/>
+      <c r="HS10" s="0"/>
+      <c r="HT10" s="0"/>
+      <c r="HU10" s="0"/>
+      <c r="HV10" s="0"/>
+      <c r="HW10" s="0"/>
+      <c r="HX10" s="0"/>
+      <c r="HY10" s="0"/>
+      <c r="HZ10" s="0"/>
+      <c r="IA10" s="0"/>
+      <c r="IB10" s="0"/>
+      <c r="IC10" s="0"/>
+      <c r="ID10" s="0"/>
+      <c r="IE10" s="0"/>
+      <c r="IF10" s="0"/>
+      <c r="IG10" s="0"/>
+      <c r="IH10" s="0"/>
+      <c r="II10" s="0"/>
+      <c r="IJ10" s="0"/>
+      <c r="IK10" s="0"/>
+      <c r="IL10" s="0"/>
+      <c r="IM10" s="0"/>
+      <c r="IN10" s="0"/>
+      <c r="IO10" s="0"/>
+      <c r="IP10" s="0"/>
+      <c r="IQ10" s="0"/>
+      <c r="IR10" s="0"/>
+      <c r="IS10" s="0"/>
+      <c r="IT10" s="0"/>
+      <c r="IU10" s="0"/>
+      <c r="IV10" s="0"/>
+      <c r="IW10" s="0"/>
+      <c r="IX10" s="0"/>
+      <c r="IY10" s="0"/>
+      <c r="IZ10" s="0"/>
+      <c r="JA10" s="0"/>
+      <c r="JB10" s="0"/>
+      <c r="JC10" s="0"/>
+      <c r="JD10" s="0"/>
+      <c r="JE10" s="0"/>
+      <c r="JF10" s="0"/>
+      <c r="JG10" s="0"/>
+      <c r="JH10" s="0"/>
+      <c r="JI10" s="0"/>
+      <c r="JJ10" s="0"/>
+      <c r="JK10" s="0"/>
+      <c r="JL10" s="0"/>
+      <c r="JM10" s="0"/>
+      <c r="JN10" s="0"/>
+      <c r="JO10" s="0"/>
+      <c r="JP10" s="0"/>
+      <c r="JQ10" s="0"/>
+      <c r="JR10" s="0"/>
+      <c r="JS10" s="0"/>
+      <c r="JT10" s="0"/>
+      <c r="JU10" s="0"/>
+      <c r="JV10" s="0"/>
+      <c r="JW10" s="0"/>
+      <c r="JX10" s="0"/>
+      <c r="JY10" s="0"/>
+      <c r="JZ10" s="0"/>
+      <c r="KA10" s="0"/>
+      <c r="KB10" s="0"/>
+      <c r="KC10" s="0"/>
+      <c r="KD10" s="0"/>
+      <c r="KE10" s="0"/>
+      <c r="KF10" s="0"/>
+      <c r="KG10" s="0"/>
+      <c r="KH10" s="0"/>
+      <c r="KI10" s="0"/>
+      <c r="KJ10" s="0"/>
+      <c r="KK10" s="0"/>
+      <c r="KL10" s="0"/>
+      <c r="KM10" s="0"/>
+      <c r="KN10" s="0"/>
+      <c r="KO10" s="0"/>
+      <c r="KP10" s="0"/>
+      <c r="KQ10" s="0"/>
+      <c r="KR10" s="0"/>
+      <c r="KS10" s="0"/>
+      <c r="KT10" s="0"/>
+      <c r="KU10" s="0"/>
+      <c r="KV10" s="0"/>
+      <c r="KW10" s="0"/>
+      <c r="KX10" s="0"/>
+      <c r="KY10" s="0"/>
+      <c r="KZ10" s="0"/>
+      <c r="LA10" s="0"/>
+      <c r="LB10" s="0"/>
+      <c r="LC10" s="0"/>
+      <c r="LD10" s="0"/>
+      <c r="LE10" s="0"/>
+      <c r="LF10" s="0"/>
+      <c r="LG10" s="0"/>
+      <c r="LH10" s="0"/>
+      <c r="LI10" s="0"/>
+      <c r="LJ10" s="0"/>
+      <c r="LK10" s="0"/>
+      <c r="LL10" s="0"/>
+      <c r="LM10" s="0"/>
+      <c r="LN10" s="0"/>
+      <c r="LO10" s="0"/>
+      <c r="LP10" s="0"/>
+      <c r="LQ10" s="0"/>
+      <c r="LR10" s="0"/>
+      <c r="LS10" s="0"/>
+      <c r="LT10" s="0"/>
+      <c r="LU10" s="0"/>
+      <c r="LV10" s="0"/>
+      <c r="LW10" s="0"/>
+      <c r="LX10" s="0"/>
+      <c r="LY10" s="0"/>
+      <c r="LZ10" s="0"/>
+      <c r="MA10" s="0"/>
+      <c r="MB10" s="0"/>
+      <c r="MC10" s="0"/>
+      <c r="MD10" s="0"/>
+      <c r="ME10" s="0"/>
+      <c r="MF10" s="0"/>
+      <c r="MG10" s="0"/>
+      <c r="MH10" s="0"/>
+      <c r="MI10" s="0"/>
+      <c r="MJ10" s="0"/>
+      <c r="MK10" s="0"/>
+      <c r="ML10" s="0"/>
+      <c r="MM10" s="0"/>
+      <c r="MN10" s="0"/>
+      <c r="MO10" s="0"/>
+      <c r="MP10" s="0"/>
+      <c r="MQ10" s="0"/>
+      <c r="MR10" s="0"/>
+      <c r="MS10" s="0"/>
+      <c r="MT10" s="0"/>
+      <c r="MU10" s="0"/>
+      <c r="MV10" s="0"/>
+      <c r="MW10" s="0"/>
+      <c r="MX10" s="0"/>
+      <c r="MY10" s="0"/>
+      <c r="MZ10" s="0"/>
+      <c r="NA10" s="0"/>
+      <c r="NB10" s="0"/>
+      <c r="NC10" s="0"/>
+      <c r="ND10" s="0"/>
+      <c r="NE10" s="0"/>
+      <c r="NF10" s="0"/>
+      <c r="NG10" s="0"/>
+      <c r="NH10" s="0"/>
+      <c r="NI10" s="0"/>
+      <c r="NJ10" s="0"/>
+      <c r="NK10" s="0"/>
+      <c r="NL10" s="0"/>
+      <c r="NM10" s="0"/>
+      <c r="NN10" s="0"/>
+      <c r="NO10" s="0"/>
+      <c r="NP10" s="0"/>
+      <c r="NQ10" s="0"/>
+      <c r="NR10" s="0"/>
+      <c r="NS10" s="0"/>
+      <c r="NT10" s="0"/>
+      <c r="NU10" s="0"/>
+      <c r="NV10" s="0"/>
+      <c r="NW10" s="0"/>
+      <c r="NX10" s="0"/>
+      <c r="NY10" s="0"/>
+      <c r="NZ10" s="0"/>
+      <c r="OA10" s="0"/>
+      <c r="OB10" s="0"/>
+      <c r="OC10" s="0"/>
+      <c r="OD10" s="0"/>
+      <c r="OE10" s="0"/>
+      <c r="OF10" s="0"/>
+      <c r="OG10" s="0"/>
+      <c r="OH10" s="0"/>
+      <c r="OI10" s="0"/>
+      <c r="OJ10" s="0"/>
+      <c r="OK10" s="0"/>
+      <c r="OL10" s="0"/>
+      <c r="OM10" s="0"/>
+      <c r="ON10" s="0"/>
+      <c r="OO10" s="0"/>
+      <c r="OP10" s="0"/>
+      <c r="OQ10" s="0"/>
+      <c r="OR10" s="0"/>
+      <c r="OS10" s="0"/>
+      <c r="OT10" s="0"/>
+      <c r="OU10" s="0"/>
+      <c r="OV10" s="0"/>
+      <c r="OW10" s="0"/>
+      <c r="OX10" s="0"/>
+      <c r="OY10" s="0"/>
+      <c r="OZ10" s="0"/>
+      <c r="PA10" s="0"/>
+      <c r="PB10" s="0"/>
+      <c r="PC10" s="0"/>
+      <c r="PD10" s="0"/>
+      <c r="PE10" s="0"/>
+      <c r="PF10" s="0"/>
+      <c r="PG10" s="0"/>
+      <c r="PH10" s="0"/>
+      <c r="PI10" s="0"/>
+      <c r="PJ10" s="0"/>
+      <c r="PK10" s="0"/>
+      <c r="PL10" s="0"/>
+      <c r="PM10" s="0"/>
+      <c r="PN10" s="0"/>
+      <c r="PO10" s="0"/>
+      <c r="PP10" s="0"/>
+      <c r="PQ10" s="0"/>
+      <c r="PR10" s="0"/>
+      <c r="PS10" s="0"/>
+      <c r="PT10" s="0"/>
+      <c r="PU10" s="0"/>
+      <c r="PV10" s="0"/>
+      <c r="PW10" s="0"/>
+      <c r="PX10" s="0"/>
+      <c r="PY10" s="0"/>
+      <c r="PZ10" s="0"/>
+      <c r="QA10" s="0"/>
+      <c r="QB10" s="0"/>
+      <c r="QC10" s="0"/>
+      <c r="QD10" s="0"/>
+      <c r="QE10" s="0"/>
+      <c r="QF10" s="0"/>
+      <c r="QG10" s="0"/>
+      <c r="QH10" s="0"/>
+      <c r="QI10" s="0"/>
+      <c r="QJ10" s="0"/>
+      <c r="QK10" s="0"/>
+      <c r="QL10" s="0"/>
+      <c r="QM10" s="0"/>
+      <c r="QN10" s="0"/>
+      <c r="QO10" s="0"/>
+      <c r="QP10" s="0"/>
+      <c r="QQ10" s="0"/>
+      <c r="QR10" s="0"/>
+      <c r="QS10" s="0"/>
+      <c r="QT10" s="0"/>
+      <c r="QU10" s="0"/>
+      <c r="QV10" s="0"/>
+      <c r="QW10" s="0"/>
+      <c r="QX10" s="0"/>
+      <c r="QY10" s="0"/>
+      <c r="QZ10" s="0"/>
+      <c r="RA10" s="0"/>
+      <c r="RB10" s="0"/>
+      <c r="RC10" s="0"/>
+      <c r="RD10" s="0"/>
+      <c r="RE10" s="0"/>
+      <c r="RF10" s="0"/>
+      <c r="RG10" s="0"/>
+      <c r="RH10" s="0"/>
+      <c r="RI10" s="0"/>
+      <c r="RJ10" s="0"/>
+      <c r="RK10" s="0"/>
+      <c r="RL10" s="0"/>
+      <c r="RM10" s="0"/>
+      <c r="RN10" s="0"/>
+      <c r="RO10" s="0"/>
+      <c r="RP10" s="0"/>
+      <c r="RQ10" s="0"/>
+      <c r="RR10" s="0"/>
+      <c r="RS10" s="0"/>
+      <c r="RT10" s="0"/>
+      <c r="RU10" s="0"/>
+      <c r="RV10" s="0"/>
+      <c r="RW10" s="0"/>
+      <c r="RX10" s="0"/>
+      <c r="RY10" s="0"/>
+      <c r="RZ10" s="0"/>
+      <c r="SA10" s="0"/>
+      <c r="SB10" s="0"/>
+      <c r="SC10" s="0"/>
+      <c r="SD10" s="0"/>
+      <c r="SE10" s="0"/>
+      <c r="SF10" s="0"/>
+      <c r="SG10" s="0"/>
+      <c r="SH10" s="0"/>
+      <c r="SI10" s="0"/>
+      <c r="SJ10" s="0"/>
+      <c r="SK10" s="0"/>
+      <c r="SL10" s="0"/>
+      <c r="SM10" s="0"/>
+      <c r="SN10" s="0"/>
+      <c r="SO10" s="0"/>
+      <c r="SP10" s="0"/>
+      <c r="SQ10" s="0"/>
+      <c r="SR10" s="0"/>
+      <c r="SS10" s="0"/>
+      <c r="ST10" s="0"/>
+      <c r="SU10" s="0"/>
+      <c r="SV10" s="0"/>
+      <c r="SW10" s="0"/>
+      <c r="SX10" s="0"/>
+      <c r="SY10" s="0"/>
+      <c r="SZ10" s="0"/>
+      <c r="TA10" s="0"/>
+      <c r="TB10" s="0"/>
+      <c r="TC10" s="0"/>
+      <c r="TD10" s="0"/>
+      <c r="TE10" s="0"/>
+      <c r="TF10" s="0"/>
+      <c r="TG10" s="0"/>
+      <c r="TH10" s="0"/>
+      <c r="TI10" s="0"/>
+      <c r="TJ10" s="0"/>
+      <c r="TK10" s="0"/>
+      <c r="TL10" s="0"/>
+      <c r="TM10" s="0"/>
+      <c r="TN10" s="0"/>
+      <c r="TO10" s="0"/>
+      <c r="TP10" s="0"/>
+      <c r="TQ10" s="0"/>
+      <c r="TR10" s="0"/>
+      <c r="TS10" s="0"/>
+      <c r="TT10" s="0"/>
+      <c r="TU10" s="0"/>
+      <c r="TV10" s="0"/>
+      <c r="TW10" s="0"/>
+      <c r="TX10" s="0"/>
+      <c r="TY10" s="0"/>
+      <c r="TZ10" s="0"/>
+      <c r="UA10" s="0"/>
+      <c r="UB10" s="0"/>
+      <c r="UC10" s="0"/>
+      <c r="UD10" s="0"/>
+      <c r="UE10" s="0"/>
+      <c r="UF10" s="0"/>
+      <c r="UG10" s="0"/>
+      <c r="UH10" s="0"/>
+      <c r="UI10" s="0"/>
+      <c r="UJ10" s="0"/>
+      <c r="UK10" s="0"/>
+      <c r="UL10" s="0"/>
+      <c r="UM10" s="0"/>
+      <c r="UN10" s="0"/>
+      <c r="UO10" s="0"/>
+      <c r="UP10" s="0"/>
+      <c r="UQ10" s="0"/>
+      <c r="UR10" s="0"/>
+      <c r="US10" s="0"/>
+      <c r="UT10" s="0"/>
+      <c r="UU10" s="0"/>
+      <c r="UV10" s="0"/>
+      <c r="UW10" s="0"/>
+      <c r="UX10" s="0"/>
+      <c r="UY10" s="0"/>
+      <c r="UZ10" s="0"/>
+      <c r="VA10" s="0"/>
+      <c r="VB10" s="0"/>
+      <c r="VC10" s="0"/>
+      <c r="VD10" s="0"/>
+      <c r="VE10" s="0"/>
+      <c r="VF10" s="0"/>
+      <c r="VG10" s="0"/>
+      <c r="VH10" s="0"/>
+      <c r="VI10" s="0"/>
+      <c r="VJ10" s="0"/>
+      <c r="VK10" s="0"/>
+      <c r="VL10" s="0"/>
+      <c r="VM10" s="0"/>
+      <c r="VN10" s="0"/>
+      <c r="VO10" s="0"/>
+      <c r="VP10" s="0"/>
+      <c r="VQ10" s="0"/>
+      <c r="VR10" s="0"/>
+      <c r="VS10" s="0"/>
+      <c r="VT10" s="0"/>
+      <c r="VU10" s="0"/>
+      <c r="VV10" s="0"/>
+      <c r="VW10" s="0"/>
+      <c r="VX10" s="0"/>
+      <c r="VY10" s="0"/>
+      <c r="VZ10" s="0"/>
+      <c r="WA10" s="0"/>
+      <c r="WB10" s="0"/>
+      <c r="WC10" s="0"/>
+      <c r="WD10" s="0"/>
+      <c r="WE10" s="0"/>
+      <c r="WF10" s="0"/>
+      <c r="WG10" s="0"/>
+      <c r="WH10" s="0"/>
+      <c r="WI10" s="0"/>
+      <c r="WJ10" s="0"/>
+      <c r="WK10" s="0"/>
+      <c r="WL10" s="0"/>
+      <c r="WM10" s="0"/>
+      <c r="WN10" s="0"/>
+      <c r="WO10" s="0"/>
+      <c r="WP10" s="0"/>
+      <c r="WQ10" s="0"/>
+      <c r="WR10" s="0"/>
+      <c r="WS10" s="0"/>
+      <c r="WT10" s="0"/>
+      <c r="WU10" s="0"/>
+      <c r="WV10" s="0"/>
+      <c r="WW10" s="0"/>
+      <c r="WX10" s="0"/>
+      <c r="WY10" s="0"/>
+      <c r="WZ10" s="0"/>
+      <c r="XA10" s="0"/>
+      <c r="XB10" s="0"/>
+      <c r="XC10" s="0"/>
+      <c r="XD10" s="0"/>
+      <c r="XE10" s="0"/>
+      <c r="XF10" s="0"/>
+      <c r="XG10" s="0"/>
+      <c r="XH10" s="0"/>
+      <c r="XI10" s="0"/>
+      <c r="XJ10" s="0"/>
+      <c r="XK10" s="0"/>
+      <c r="XL10" s="0"/>
+      <c r="XM10" s="0"/>
+      <c r="XN10" s="0"/>
+      <c r="XO10" s="0"/>
+      <c r="XP10" s="0"/>
+      <c r="XQ10" s="0"/>
+      <c r="XR10" s="0"/>
+      <c r="XS10" s="0"/>
+      <c r="XT10" s="0"/>
+      <c r="XU10" s="0"/>
+      <c r="XV10" s="0"/>
+      <c r="XW10" s="0"/>
+      <c r="XX10" s="0"/>
+      <c r="XY10" s="0"/>
+      <c r="XZ10" s="0"/>
+      <c r="YA10" s="0"/>
+      <c r="YB10" s="0"/>
+      <c r="YC10" s="0"/>
+      <c r="YD10" s="0"/>
+      <c r="YE10" s="0"/>
+      <c r="YF10" s="0"/>
+      <c r="YG10" s="0"/>
+      <c r="YH10" s="0"/>
+      <c r="YI10" s="0"/>
+      <c r="YJ10" s="0"/>
+      <c r="YK10" s="0"/>
+      <c r="YL10" s="0"/>
+      <c r="YM10" s="0"/>
+      <c r="YN10" s="0"/>
+      <c r="YO10" s="0"/>
+      <c r="YP10" s="0"/>
+      <c r="YQ10" s="0"/>
+      <c r="YR10" s="0"/>
+      <c r="YS10" s="0"/>
+      <c r="YT10" s="0"/>
+      <c r="YU10" s="0"/>
+      <c r="YV10" s="0"/>
+      <c r="YW10" s="0"/>
+      <c r="YX10" s="0"/>
+      <c r="YY10" s="0"/>
+      <c r="YZ10" s="0"/>
+      <c r="ZA10" s="0"/>
+      <c r="ZB10" s="0"/>
+      <c r="ZC10" s="0"/>
+      <c r="ZD10" s="0"/>
+      <c r="ZE10" s="0"/>
+      <c r="ZF10" s="0"/>
+      <c r="ZG10" s="0"/>
+      <c r="ZH10" s="0"/>
+      <c r="ZI10" s="0"/>
+      <c r="ZJ10" s="0"/>
+      <c r="ZK10" s="0"/>
+      <c r="ZL10" s="0"/>
+      <c r="ZM10" s="0"/>
+      <c r="ZN10" s="0"/>
+      <c r="ZO10" s="0"/>
+      <c r="ZP10" s="0"/>
+      <c r="ZQ10" s="0"/>
+      <c r="ZR10" s="0"/>
+      <c r="ZS10" s="0"/>
+      <c r="ZT10" s="0"/>
+      <c r="ZU10" s="0"/>
+      <c r="ZV10" s="0"/>
+      <c r="ZW10" s="0"/>
+      <c r="ZX10" s="0"/>
+      <c r="ZY10" s="0"/>
+      <c r="ZZ10" s="0"/>
+      <c r="AAA10" s="0"/>
+      <c r="AAB10" s="0"/>
+      <c r="AAC10" s="0"/>
+      <c r="AAD10" s="0"/>
+      <c r="AAE10" s="0"/>
+      <c r="AAF10" s="0"/>
+      <c r="AAG10" s="0"/>
+      <c r="AAH10" s="0"/>
+      <c r="AAI10" s="0"/>
+      <c r="AAJ10" s="0"/>
+      <c r="AAK10" s="0"/>
+      <c r="AAL10" s="0"/>
+      <c r="AAM10" s="0"/>
+      <c r="AAN10" s="0"/>
+      <c r="AAO10" s="0"/>
+      <c r="AAP10" s="0"/>
+      <c r="AAQ10" s="0"/>
+      <c r="AAR10" s="0"/>
+      <c r="AAS10" s="0"/>
+      <c r="AAT10" s="0"/>
+      <c r="AAU10" s="0"/>
+      <c r="AAV10" s="0"/>
+      <c r="AAW10" s="0"/>
+      <c r="AAX10" s="0"/>
+      <c r="AAY10" s="0"/>
+      <c r="AAZ10" s="0"/>
+      <c r="ABA10" s="0"/>
+      <c r="ABB10" s="0"/>
+      <c r="ABC10" s="0"/>
+      <c r="ABD10" s="0"/>
+      <c r="ABE10" s="0"/>
+      <c r="ABF10" s="0"/>
+      <c r="ABG10" s="0"/>
+      <c r="ABH10" s="0"/>
+      <c r="ABI10" s="0"/>
+      <c r="ABJ10" s="0"/>
+      <c r="ABK10" s="0"/>
+      <c r="ABL10" s="0"/>
+      <c r="ABM10" s="0"/>
+      <c r="ABN10" s="0"/>
+      <c r="ABO10" s="0"/>
+      <c r="ABP10" s="0"/>
+      <c r="ABQ10" s="0"/>
+      <c r="ABR10" s="0"/>
+      <c r="ABS10" s="0"/>
+      <c r="ABT10" s="0"/>
+      <c r="ABU10" s="0"/>
+      <c r="ABV10" s="0"/>
+      <c r="ABW10" s="0"/>
+      <c r="ABX10" s="0"/>
+      <c r="ABY10" s="0"/>
+      <c r="ABZ10" s="0"/>
+      <c r="ACA10" s="0"/>
+      <c r="ACB10" s="0"/>
+      <c r="ACC10" s="0"/>
+      <c r="ACD10" s="0"/>
+      <c r="ACE10" s="0"/>
+      <c r="ACF10" s="0"/>
+      <c r="ACG10" s="0"/>
+      <c r="ACH10" s="0"/>
+      <c r="ACI10" s="0"/>
+      <c r="ACJ10" s="0"/>
+      <c r="ACK10" s="0"/>
+      <c r="ACL10" s="0"/>
+      <c r="ACM10" s="0"/>
+      <c r="ACN10" s="0"/>
+      <c r="ACO10" s="0"/>
+      <c r="ACP10" s="0"/>
+      <c r="ACQ10" s="0"/>
+      <c r="ACR10" s="0"/>
+      <c r="ACS10" s="0"/>
+      <c r="ACT10" s="0"/>
+      <c r="ACU10" s="0"/>
+      <c r="ACV10" s="0"/>
+      <c r="ACW10" s="0"/>
+      <c r="ACX10" s="0"/>
+      <c r="ACY10" s="0"/>
+      <c r="ACZ10" s="0"/>
+      <c r="ADA10" s="0"/>
+      <c r="ADB10" s="0"/>
+      <c r="ADC10" s="0"/>
+      <c r="ADD10" s="0"/>
+      <c r="ADE10" s="0"/>
+      <c r="ADF10" s="0"/>
+      <c r="ADG10" s="0"/>
+      <c r="ADH10" s="0"/>
+      <c r="ADI10" s="0"/>
+      <c r="ADJ10" s="0"/>
+      <c r="ADK10" s="0"/>
+      <c r="ADL10" s="0"/>
+      <c r="ADM10" s="0"/>
+      <c r="ADN10" s="0"/>
+      <c r="ADO10" s="0"/>
+      <c r="ADP10" s="0"/>
+      <c r="ADQ10" s="0"/>
+      <c r="ADR10" s="0"/>
+      <c r="ADS10" s="0"/>
+      <c r="ADT10" s="0"/>
+      <c r="ADU10" s="0"/>
+      <c r="ADV10" s="0"/>
+      <c r="ADW10" s="0"/>
+      <c r="ADX10" s="0"/>
+      <c r="ADY10" s="0"/>
+      <c r="ADZ10" s="0"/>
+      <c r="AEA10" s="0"/>
+      <c r="AEB10" s="0"/>
+      <c r="AEC10" s="0"/>
+      <c r="AED10" s="0"/>
+      <c r="AEE10" s="0"/>
+      <c r="AEF10" s="0"/>
+      <c r="AEG10" s="0"/>
+      <c r="AEH10" s="0"/>
+      <c r="AEI10" s="0"/>
+      <c r="AEJ10" s="0"/>
+      <c r="AEK10" s="0"/>
+      <c r="AEL10" s="0"/>
+      <c r="AEM10" s="0"/>
+      <c r="AEN10" s="0"/>
+      <c r="AEO10" s="0"/>
+      <c r="AEP10" s="0"/>
+      <c r="AEQ10" s="0"/>
+      <c r="AER10" s="0"/>
+      <c r="AES10" s="0"/>
+      <c r="AET10" s="0"/>
+      <c r="AEU10" s="0"/>
+      <c r="AEV10" s="0"/>
+      <c r="AEW10" s="0"/>
+      <c r="AEX10" s="0"/>
+      <c r="AEY10" s="0"/>
+      <c r="AEZ10" s="0"/>
+      <c r="AFA10" s="0"/>
+      <c r="AFB10" s="0"/>
+      <c r="AFC10" s="0"/>
+      <c r="AFD10" s="0"/>
+      <c r="AFE10" s="0"/>
+      <c r="AFF10" s="0"/>
+      <c r="AFG10" s="0"/>
+      <c r="AFH10" s="0"/>
+      <c r="AFI10" s="0"/>
+      <c r="AFJ10" s="0"/>
+      <c r="AFK10" s="0"/>
+      <c r="AFL10" s="0"/>
+      <c r="AFM10" s="0"/>
+      <c r="AFN10" s="0"/>
+      <c r="AFO10" s="0"/>
+      <c r="AFP10" s="0"/>
+      <c r="AFQ10" s="0"/>
+      <c r="AFR10" s="0"/>
+      <c r="AFS10" s="0"/>
+      <c r="AFT10" s="0"/>
+      <c r="AFU10" s="0"/>
+      <c r="AFV10" s="0"/>
+      <c r="AFW10" s="0"/>
+      <c r="AFX10" s="0"/>
+      <c r="AFY10" s="0"/>
+      <c r="AFZ10" s="0"/>
+      <c r="AGA10" s="0"/>
+      <c r="AGB10" s="0"/>
+      <c r="AGC10" s="0"/>
+      <c r="AGD10" s="0"/>
+      <c r="AGE10" s="0"/>
+      <c r="AGF10" s="0"/>
+      <c r="AGG10" s="0"/>
+      <c r="AGH10" s="0"/>
+      <c r="AGI10" s="0"/>
+      <c r="AGJ10" s="0"/>
+      <c r="AGK10" s="0"/>
+      <c r="AGL10" s="0"/>
+      <c r="AGM10" s="0"/>
+      <c r="AGN10" s="0"/>
+      <c r="AGO10" s="0"/>
+      <c r="AGP10" s="0"/>
+      <c r="AGQ10" s="0"/>
+      <c r="AGR10" s="0"/>
+      <c r="AGS10" s="0"/>
+      <c r="AGT10" s="0"/>
+      <c r="AGU10" s="0"/>
+      <c r="AGV10" s="0"/>
+      <c r="AGW10" s="0"/>
+      <c r="AGX10" s="0"/>
+      <c r="AGY10" s="0"/>
+      <c r="AGZ10" s="0"/>
+      <c r="AHA10" s="0"/>
+      <c r="AHB10" s="0"/>
+      <c r="AHC10" s="0"/>
+      <c r="AHD10" s="0"/>
+      <c r="AHE10" s="0"/>
+      <c r="AHF10" s="0"/>
+      <c r="AHG10" s="0"/>
+      <c r="AHH10" s="0"/>
+      <c r="AHI10" s="0"/>
+      <c r="AHJ10" s="0"/>
+      <c r="AHK10" s="0"/>
+      <c r="AHL10" s="0"/>
+      <c r="AHM10" s="0"/>
+      <c r="AHN10" s="0"/>
+      <c r="AHO10" s="0"/>
+      <c r="AHP10" s="0"/>
+      <c r="AHQ10" s="0"/>
+      <c r="AHR10" s="0"/>
+      <c r="AHS10" s="0"/>
+      <c r="AHT10" s="0"/>
+      <c r="AHU10" s="0"/>
+      <c r="AHV10" s="0"/>
+      <c r="AHW10" s="0"/>
+      <c r="AHX10" s="0"/>
+      <c r="AHY10" s="0"/>
+      <c r="AHZ10" s="0"/>
+      <c r="AIA10" s="0"/>
+      <c r="AIB10" s="0"/>
+      <c r="AIC10" s="0"/>
+      <c r="AID10" s="0"/>
+      <c r="AIE10" s="0"/>
+      <c r="AIF10" s="0"/>
+      <c r="AIG10" s="0"/>
+      <c r="AIH10" s="0"/>
+      <c r="AII10" s="0"/>
+      <c r="AIJ10" s="0"/>
+      <c r="AIK10" s="0"/>
+      <c r="AIL10" s="0"/>
+      <c r="AIM10" s="0"/>
+      <c r="AIN10" s="0"/>
+      <c r="AIO10" s="0"/>
+      <c r="AIP10" s="0"/>
+      <c r="AIQ10" s="0"/>
+      <c r="AIR10" s="0"/>
+      <c r="AIS10" s="0"/>
+      <c r="AIT10" s="0"/>
+      <c r="AIU10" s="0"/>
+      <c r="AIV10" s="0"/>
+      <c r="AIW10" s="0"/>
+      <c r="AIX10" s="0"/>
+      <c r="AIY10" s="0"/>
+      <c r="AIZ10" s="0"/>
+      <c r="AJA10" s="0"/>
+      <c r="AJB10" s="0"/>
+      <c r="AJC10" s="0"/>
+      <c r="AJD10" s="0"/>
+      <c r="AJE10" s="0"/>
+      <c r="AJF10" s="0"/>
+      <c r="AJG10" s="0"/>
+      <c r="AJH10" s="0"/>
+      <c r="AJI10" s="0"/>
+      <c r="AJJ10" s="0"/>
+      <c r="AJK10" s="0"/>
+      <c r="AJL10" s="0"/>
+      <c r="AJM10" s="0"/>
+      <c r="AJN10" s="0"/>
+      <c r="AJO10" s="0"/>
+      <c r="AJP10" s="0"/>
+      <c r="AJQ10" s="0"/>
+      <c r="AJR10" s="0"/>
+      <c r="AJS10" s="0"/>
+      <c r="AJT10" s="0"/>
+      <c r="AJU10" s="0"/>
+      <c r="AJV10" s="0"/>
+      <c r="AJW10" s="0"/>
+      <c r="AJX10" s="0"/>
+      <c r="AJY10" s="0"/>
+      <c r="AJZ10" s="0"/>
+      <c r="AKA10" s="0"/>
+      <c r="AKB10" s="0"/>
+      <c r="AKC10" s="0"/>
+      <c r="AKD10" s="0"/>
+      <c r="AKE10" s="0"/>
+      <c r="AKF10" s="0"/>
+      <c r="AKG10" s="0"/>
+      <c r="AKH10" s="0"/>
+      <c r="AKI10" s="0"/>
+      <c r="AKJ10" s="0"/>
+      <c r="AKK10" s="0"/>
+      <c r="AKL10" s="0"/>
+      <c r="AKM10" s="0"/>
+      <c r="AKN10" s="0"/>
+      <c r="AKO10" s="0"/>
+      <c r="AKP10" s="0"/>
+      <c r="AKQ10" s="0"/>
+      <c r="AKR10" s="0"/>
+      <c r="AKS10" s="0"/>
+      <c r="AKT10" s="0"/>
+      <c r="AKU10" s="0"/>
+      <c r="AKV10" s="0"/>
+      <c r="AKW10" s="0"/>
+      <c r="AKX10" s="0"/>
+      <c r="AKY10" s="0"/>
+      <c r="AKZ10" s="0"/>
+      <c r="ALA10" s="0"/>
+      <c r="ALB10" s="0"/>
+      <c r="ALC10" s="0"/>
+      <c r="ALD10" s="0"/>
+      <c r="ALE10" s="0"/>
+      <c r="ALF10" s="0"/>
+      <c r="ALG10" s="0"/>
+      <c r="ALH10" s="0"/>
+      <c r="ALI10" s="0"/>
+      <c r="ALJ10" s="0"/>
+      <c r="ALK10" s="0"/>
+      <c r="ALL10" s="0"/>
+      <c r="ALM10" s="0"/>
+      <c r="ALN10" s="0"/>
+      <c r="ALO10" s="0"/>
+      <c r="ALP10" s="0"/>
+      <c r="ALQ10" s="0"/>
+      <c r="ALR10" s="0"/>
+      <c r="ALS10" s="0"/>
+      <c r="ALT10" s="0"/>
+      <c r="ALU10" s="0"/>
+      <c r="ALV10" s="0"/>
+      <c r="ALW10" s="0"/>
+      <c r="ALX10" s="0"/>
+      <c r="ALY10" s="0"/>
+      <c r="ALZ10" s="0"/>
+      <c r="AMA10" s="0"/>
+      <c r="AMB10" s="0"/>
+      <c r="AMC10" s="0"/>
+      <c r="AMD10" s="0"/>
+      <c r="AME10" s="0"/>
+      <c r="AMF10" s="0"/>
+      <c r="AMG10" s="0"/>
+      <c r="AMH10" s="0"/>
+      <c r="AMI10" s="0"/>
+      <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5" t="s">
+    <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="F13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="I11" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="J11" s="3" t="n">
+      <c r="G13" s="7"/>
+      <c r="H13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="K13" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    <row r="14" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="F14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3" t="n">
+      <c r="G14" s="7"/>
+      <c r="H14" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="K14" s="3"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="1" t="n">
-        <v>107.5</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I15" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="K18" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9411,20 +11567,20 @@
   </sheetPr>
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K75" activeCellId="0" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="10" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="10" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9434,7 +11590,7 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
       <c r="F1" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
@@ -9448,37 +11604,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E3" s="17" t="n">
         <v>390</v>
@@ -9496,10 +11652,10 @@
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" s="19" t="n">
         <v>9555589203096</v>
@@ -9519,10 +11675,10 @@
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="19" t="n">
         <v>9555589203287</v>
@@ -9542,10 +11698,10 @@
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C6" s="19" t="n">
         <v>9555589200415</v>
@@ -9567,10 +11723,10 @@
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="19" t="n">
         <v>9555589203348</v>
@@ -9592,10 +11748,10 @@
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="19" t="n">
         <v>9555589200385</v>
@@ -9617,14 +11773,14 @@
     </row>
     <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E9" s="17" t="n">
         <v>390</v>
@@ -9644,14 +11800,14 @@
     </row>
     <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E10" s="17" t="n">
         <v>1.25</v>
@@ -9671,10 +11827,10 @@
     </row>
     <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C11" s="19" t="n">
         <v>9555589203294</v>
@@ -9696,10 +11852,10 @@
     </row>
     <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C12" s="19" t="n">
         <v>9555589203102</v>
@@ -9721,14 +11877,14 @@
     </row>
     <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E13" s="17" t="n">
         <v>315</v>
@@ -9748,14 +11904,14 @@
     </row>
     <row r="14" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E14" s="17" t="n">
         <v>350</v>
@@ -9775,14 +11931,14 @@
     </row>
     <row r="15" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E15" s="17" t="n">
         <v>500</v>
@@ -9796,14 +11952,14 @@
     </row>
     <row r="16" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E16" s="17" t="n">
         <v>1.5</v>
@@ -9817,14 +11973,14 @@
     </row>
     <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E17" s="17" t="n">
         <v>1</v>
@@ -9838,10 +11994,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" s="23" t="n">
         <v>9555589203287</v>
@@ -9861,10 +12017,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C19" s="23" t="n">
         <v>9555589200385</v>
@@ -9884,10 +12040,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" s="23" t="n">
         <v>9555589203096</v>
@@ -9907,10 +12063,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C21" s="23" t="n">
         <v>9555589203294</v>
@@ -9930,10 +12086,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C22" s="23" t="n">
         <v>9555589200668</v>
@@ -9953,14 +12109,14 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E23" s="18" t="n">
         <v>390</v>
@@ -9978,10 +12134,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C24" s="23" t="n">
         <v>8888002087005</v>
@@ -10001,10 +12157,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C25" s="23" t="n">
         <v>9555589200415</v>
@@ -10024,10 +12180,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C26" s="23" t="n">
         <v>9555589203102</v>
@@ -10047,14 +12203,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E27" s="18" t="n">
         <v>390</v>
@@ -10072,14 +12228,14 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E28" s="18" t="n">
         <v>1.25</v>
@@ -10093,10 +12249,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C29" s="23" t="n">
         <v>9555589200392</v>
@@ -10112,14 +12268,14 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E30" s="18" t="n">
         <v>315</v>
@@ -10137,14 +12293,14 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E31" s="18" t="n">
         <v>350</v>
@@ -10162,14 +12318,14 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E32" s="18" t="n">
         <v>500</v>
@@ -10183,10 +12339,10 @@
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C33" s="24" t="n">
         <v>9555589200385</v>
@@ -10207,10 +12363,10 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" s="26" t="n">
         <v>9555589200668</v>
@@ -10231,14 +12387,14 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E35" s="18" t="n">
         <v>330</v>
@@ -10257,14 +12413,14 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E36" s="18" t="n">
         <v>315</v>
@@ -10283,14 +12439,14 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E37" s="18" t="n">
         <v>350</v>
@@ -10309,14 +12465,14 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E38" s="18" t="n">
         <v>330</v>
@@ -10331,10 +12487,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C39" s="27" t="n">
         <v>8888002087005</v>
@@ -10351,10 +12507,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C40" s="23" t="n">
         <v>9555589200415</v>
@@ -10370,10 +12526,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C41" s="23" t="n">
         <v>9555589200699</v>
@@ -10389,10 +12545,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C42" s="23" t="n">
         <v>9555589200392</v>
@@ -10408,10 +12564,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C43" s="23" t="n">
         <v>9555589200385</v>
@@ -10427,14 +12583,14 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E44" s="18" t="n">
         <v>1.5</v>
@@ -10448,10 +12604,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C45" s="23" t="n">
         <v>9555589200644</v>
@@ -10467,14 +12623,14 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E46" s="18" t="n">
         <v>1.5</v>
@@ -10488,10 +12644,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C47" s="23" t="n">
         <v>9555589200675</v>
@@ -10507,10 +12663,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C48" s="23" t="n">
         <v>9555589200637</v>
@@ -10526,14 +12682,14 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E49" s="18" t="n">
         <v>500</v>
@@ -10547,14 +12703,14 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E50" s="18" t="n">
         <v>500</v>
@@ -10568,14 +12724,14 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E51" s="18" t="n">
         <v>500</v>
@@ -10589,14 +12745,14 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C52" s="23"/>
       <c r="D52" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E52" s="18" t="n">
         <v>350</v>
@@ -10610,14 +12766,14 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C53" s="23"/>
       <c r="D53" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E53" s="18" t="n">
         <v>1.5</v>
@@ -10631,14 +12787,14 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C54" s="23"/>
       <c r="D54" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E54" s="18" t="n">
         <v>1</v>
@@ -10652,10 +12808,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C55" s="23" t="n">
         <v>9555589203287</v>
@@ -10671,10 +12827,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C56" s="23" t="n">
         <v>9555589200415</v>
@@ -10690,10 +12846,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C57" s="23" t="n">
         <v>9555589203096</v>
@@ -10709,10 +12865,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C58" s="23" t="n">
         <v>9555589203102</v>
@@ -10728,14 +12884,14 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C59" s="23"/>
       <c r="D59" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E59" s="18" t="n">
         <v>1.25</v>
@@ -10749,10 +12905,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C60" s="23" t="n">
         <v>9555589203348</v>
@@ -10768,10 +12924,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C61" s="23" t="n">
         <v>9555589203294</v>
@@ -10787,14 +12943,14 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="18" t="s">
         <v>89</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>87</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E62" s="18" t="n">
         <v>500</v>
@@ -10808,10 +12964,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C63" s="23" t="n">
         <v>9555589200385</v>
@@ -10827,14 +12983,14 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C64" s="23"/>
       <c r="D64" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E64" s="18" t="n">
         <v>390</v>
@@ -10848,14 +13004,14 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C65" s="23"/>
       <c r="D65" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E65" s="18" t="n">
         <v>1.25</v>
@@ -10869,14 +13025,14 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C66" s="23"/>
       <c r="D66" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E66" s="18" t="n">
         <v>1.5</v>
@@ -10890,14 +13046,14 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C67" s="23"/>
       <c r="D67" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E67" s="18" t="n">
         <v>1</v>
@@ -10911,14 +13067,14 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C68" s="23"/>
       <c r="D68" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E68" s="18" t="n">
         <v>350</v>
@@ -10932,14 +13088,14 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C69" s="23"/>
       <c r="D69" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E69" s="18" t="n">
         <v>500</v>
@@ -10953,10 +13109,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C70" s="23" t="n">
         <v>9555589200415</v>
@@ -10972,10 +13128,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C71" s="23" t="n">
         <v>9555589200392</v>
@@ -10991,14 +13147,14 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C72" s="23"/>
       <c r="D72" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E72" s="18" t="n">
         <v>500</v>
@@ -11012,10 +13168,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C73" s="23" t="n">
         <v>9555589200699</v>
@@ -11031,10 +13187,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C74" s="23" t="n">
         <v>9555589200644</v>
@@ -11050,14 +13206,14 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C75" s="23"/>
       <c r="D75" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E75" s="18" t="n">
         <v>1.5</v>
@@ -11071,10 +13227,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C76" s="23" t="n">
         <v>9555589200675</v>
@@ -11090,14 +13246,14 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C77" s="23"/>
       <c r="D77" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E77" s="18" t="n">
         <v>500</v>
@@ -11111,14 +13267,14 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C78" s="23"/>
       <c r="D78" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E78" s="18" t="n">
         <v>500</v>
@@ -11132,10 +13288,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C79" s="23" t="n">
         <v>8888002087470</v>
@@ -11151,10 +13307,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C80" s="23" t="n">
         <v>9555589200385</v>
@@ -11170,14 +13326,14 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E81" s="18" t="n">
         <v>500</v>
@@ -11191,14 +13347,14 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C82" s="23"/>
       <c r="D82" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E82" s="18" t="n">
         <v>1.5</v>
@@ -11212,14 +13368,14 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C83" s="23"/>
       <c r="D83" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E83" s="18" t="n">
         <v>1</v>
@@ -11233,14 +13389,14 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C84" s="23"/>
       <c r="D84" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E84" s="18" t="n">
         <v>350</v>
@@ -11254,10 +13410,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C85" s="23" t="n">
         <v>9555589200415</v>
@@ -11273,10 +13429,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C86" s="23" t="n">
         <v>9555589200392</v>
@@ -11292,10 +13448,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C87" s="23" t="n">
         <v>9555589200385</v>
@@ -11311,10 +13467,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C88" s="23" t="n">
         <v>9555589200637</v>
@@ -11330,10 +13486,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C89" s="23" t="n">
         <v>8888002087470</v>
@@ -11349,10 +13505,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C90" s="23" t="n">
         <v>9555589200316</v>
@@ -11368,14 +13524,14 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B91" s="18" t="s">
         <v>95</v>
-      </c>
-      <c r="B91" s="18" t="s">
-        <v>93</v>
       </c>
       <c r="C91" s="23"/>
       <c r="D91" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E91" s="18" t="n">
         <v>500</v>
@@ -11389,10 +13545,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C92" s="23" t="n">
         <v>9555589200521</v>
@@ -11408,14 +13564,14 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C93" s="23"/>
       <c r="D93" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E93" s="18" t="n">
         <v>500</v>
@@ -11429,10 +13585,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C94" s="23" t="n">
         <v>9555589200675</v>
@@ -11448,14 +13604,14 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C95" s="23"/>
       <c r="D95" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E95" s="18" t="n">
         <v>500</v>
@@ -11469,10 +13625,10 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C96" s="23" t="n">
         <v>9555589200620</v>
@@ -11488,14 +13644,14 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C97" s="23"/>
       <c r="D97" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E97" s="18" t="n">
         <v>350</v>
@@ -11509,14 +13665,14 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C98" s="23"/>
       <c r="D98" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E98" s="18" t="n">
         <v>1</v>
@@ -11530,14 +13686,14 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C99" s="23"/>
       <c r="D99" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E99" s="18" t="n">
         <v>500</v>
@@ -11550,7 +13706,7 @@
       <c r="I99" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E99"/>
+  <autoFilter ref="A2:E2"/>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>

</xml_diff>

<commit_message>
PROS-12225 - CCMY KPI Pure Shelves bug fix
</commit_message>
<xml_diff>
--- a/Projects/CCMY/Data/Template.xlsx
+++ b/Projects/CCMY/Data/Template.xlsx
@@ -35,7 +35,9 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$99</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Availability!$A$2:$E$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="103">
   <si>
     <t xml:space="preserve">Store Type</t>
   </si>
@@ -131,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">CCRM Cooler Total Number of Shelves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHELF_PURITY</t>
   </si>
   <si>
     <t xml:space="preserve">CCRM Cooler (Before)</t>
@@ -879,26 +884,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:18"/>
+  <dimension ref="1:17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11325,10 +11330,10 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>26</v>
@@ -11337,7 +11342,7 @@
         <v>26</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
@@ -11351,11 +11356,1024 @@
         <v>0</v>
       </c>
       <c r="K11" s="7"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
+      <c r="Q11" s="0"/>
+      <c r="R11" s="0"/>
+      <c r="S11" s="0"/>
+      <c r="T11" s="0"/>
+      <c r="U11" s="0"/>
+      <c r="V11" s="0"/>
+      <c r="W11" s="0"/>
+      <c r="X11" s="0"/>
+      <c r="Y11" s="0"/>
+      <c r="Z11" s="0"/>
+      <c r="AA11" s="0"/>
+      <c r="AB11" s="0"/>
+      <c r="AC11" s="0"/>
+      <c r="AD11" s="0"/>
+      <c r="AE11" s="0"/>
+      <c r="AF11" s="0"/>
+      <c r="AG11" s="0"/>
+      <c r="AH11" s="0"/>
+      <c r="AI11" s="0"/>
+      <c r="AJ11" s="0"/>
+      <c r="AK11" s="0"/>
+      <c r="AL11" s="0"/>
+      <c r="AM11" s="0"/>
+      <c r="AN11" s="0"/>
+      <c r="AO11" s="0"/>
+      <c r="AP11" s="0"/>
+      <c r="AQ11" s="0"/>
+      <c r="AR11" s="0"/>
+      <c r="AS11" s="0"/>
+      <c r="AT11" s="0"/>
+      <c r="AU11" s="0"/>
+      <c r="AV11" s="0"/>
+      <c r="AW11" s="0"/>
+      <c r="AX11" s="0"/>
+      <c r="AY11" s="0"/>
+      <c r="AZ11" s="0"/>
+      <c r="BA11" s="0"/>
+      <c r="BB11" s="0"/>
+      <c r="BC11" s="0"/>
+      <c r="BD11" s="0"/>
+      <c r="BE11" s="0"/>
+      <c r="BF11" s="0"/>
+      <c r="BG11" s="0"/>
+      <c r="BH11" s="0"/>
+      <c r="BI11" s="0"/>
+      <c r="BJ11" s="0"/>
+      <c r="BK11" s="0"/>
+      <c r="BL11" s="0"/>
+      <c r="BM11" s="0"/>
+      <c r="BN11" s="0"/>
+      <c r="BO11" s="0"/>
+      <c r="BP11" s="0"/>
+      <c r="BQ11" s="0"/>
+      <c r="BR11" s="0"/>
+      <c r="BS11" s="0"/>
+      <c r="BT11" s="0"/>
+      <c r="BU11" s="0"/>
+      <c r="BV11" s="0"/>
+      <c r="BW11" s="0"/>
+      <c r="BX11" s="0"/>
+      <c r="BY11" s="0"/>
+      <c r="BZ11" s="0"/>
+      <c r="CA11" s="0"/>
+      <c r="CB11" s="0"/>
+      <c r="CC11" s="0"/>
+      <c r="CD11" s="0"/>
+      <c r="CE11" s="0"/>
+      <c r="CF11" s="0"/>
+      <c r="CG11" s="0"/>
+      <c r="CH11" s="0"/>
+      <c r="CI11" s="0"/>
+      <c r="CJ11" s="0"/>
+      <c r="CK11" s="0"/>
+      <c r="CL11" s="0"/>
+      <c r="CM11" s="0"/>
+      <c r="CN11" s="0"/>
+      <c r="CO11" s="0"/>
+      <c r="CP11" s="0"/>
+      <c r="CQ11" s="0"/>
+      <c r="CR11" s="0"/>
+      <c r="CS11" s="0"/>
+      <c r="CT11" s="0"/>
+      <c r="CU11" s="0"/>
+      <c r="CV11" s="0"/>
+      <c r="CW11" s="0"/>
+      <c r="CX11" s="0"/>
+      <c r="CY11" s="0"/>
+      <c r="CZ11" s="0"/>
+      <c r="DA11" s="0"/>
+      <c r="DB11" s="0"/>
+      <c r="DC11" s="0"/>
+      <c r="DD11" s="0"/>
+      <c r="DE11" s="0"/>
+      <c r="DF11" s="0"/>
+      <c r="DG11" s="0"/>
+      <c r="DH11" s="0"/>
+      <c r="DI11" s="0"/>
+      <c r="DJ11" s="0"/>
+      <c r="DK11" s="0"/>
+      <c r="DL11" s="0"/>
+      <c r="DM11" s="0"/>
+      <c r="DN11" s="0"/>
+      <c r="DO11" s="0"/>
+      <c r="DP11" s="0"/>
+      <c r="DQ11" s="0"/>
+      <c r="DR11" s="0"/>
+      <c r="DS11" s="0"/>
+      <c r="DT11" s="0"/>
+      <c r="DU11" s="0"/>
+      <c r="DV11" s="0"/>
+      <c r="DW11" s="0"/>
+      <c r="DX11" s="0"/>
+      <c r="DY11" s="0"/>
+      <c r="DZ11" s="0"/>
+      <c r="EA11" s="0"/>
+      <c r="EB11" s="0"/>
+      <c r="EC11" s="0"/>
+      <c r="ED11" s="0"/>
+      <c r="EE11" s="0"/>
+      <c r="EF11" s="0"/>
+      <c r="EG11" s="0"/>
+      <c r="EH11" s="0"/>
+      <c r="EI11" s="0"/>
+      <c r="EJ11" s="0"/>
+      <c r="EK11" s="0"/>
+      <c r="EL11" s="0"/>
+      <c r="EM11" s="0"/>
+      <c r="EN11" s="0"/>
+      <c r="EO11" s="0"/>
+      <c r="EP11" s="0"/>
+      <c r="EQ11" s="0"/>
+      <c r="ER11" s="0"/>
+      <c r="ES11" s="0"/>
+      <c r="ET11" s="0"/>
+      <c r="EU11" s="0"/>
+      <c r="EV11" s="0"/>
+      <c r="EW11" s="0"/>
+      <c r="EX11" s="0"/>
+      <c r="EY11" s="0"/>
+      <c r="EZ11" s="0"/>
+      <c r="FA11" s="0"/>
+      <c r="FB11" s="0"/>
+      <c r="FC11" s="0"/>
+      <c r="FD11" s="0"/>
+      <c r="FE11" s="0"/>
+      <c r="FF11" s="0"/>
+      <c r="FG11" s="0"/>
+      <c r="FH11" s="0"/>
+      <c r="FI11" s="0"/>
+      <c r="FJ11" s="0"/>
+      <c r="FK11" s="0"/>
+      <c r="FL11" s="0"/>
+      <c r="FM11" s="0"/>
+      <c r="FN11" s="0"/>
+      <c r="FO11" s="0"/>
+      <c r="FP11" s="0"/>
+      <c r="FQ11" s="0"/>
+      <c r="FR11" s="0"/>
+      <c r="FS11" s="0"/>
+      <c r="FT11" s="0"/>
+      <c r="FU11" s="0"/>
+      <c r="FV11" s="0"/>
+      <c r="FW11" s="0"/>
+      <c r="FX11" s="0"/>
+      <c r="FY11" s="0"/>
+      <c r="FZ11" s="0"/>
+      <c r="GA11" s="0"/>
+      <c r="GB11" s="0"/>
+      <c r="GC11" s="0"/>
+      <c r="GD11" s="0"/>
+      <c r="GE11" s="0"/>
+      <c r="GF11" s="0"/>
+      <c r="GG11" s="0"/>
+      <c r="GH11" s="0"/>
+      <c r="GI11" s="0"/>
+      <c r="GJ11" s="0"/>
+      <c r="GK11" s="0"/>
+      <c r="GL11" s="0"/>
+      <c r="GM11" s="0"/>
+      <c r="GN11" s="0"/>
+      <c r="GO11" s="0"/>
+      <c r="GP11" s="0"/>
+      <c r="GQ11" s="0"/>
+      <c r="GR11" s="0"/>
+      <c r="GS11" s="0"/>
+      <c r="GT11" s="0"/>
+      <c r="GU11" s="0"/>
+      <c r="GV11" s="0"/>
+      <c r="GW11" s="0"/>
+      <c r="GX11" s="0"/>
+      <c r="GY11" s="0"/>
+      <c r="GZ11" s="0"/>
+      <c r="HA11" s="0"/>
+      <c r="HB11" s="0"/>
+      <c r="HC11" s="0"/>
+      <c r="HD11" s="0"/>
+      <c r="HE11" s="0"/>
+      <c r="HF11" s="0"/>
+      <c r="HG11" s="0"/>
+      <c r="HH11" s="0"/>
+      <c r="HI11" s="0"/>
+      <c r="HJ11" s="0"/>
+      <c r="HK11" s="0"/>
+      <c r="HL11" s="0"/>
+      <c r="HM11" s="0"/>
+      <c r="HN11" s="0"/>
+      <c r="HO11" s="0"/>
+      <c r="HP11" s="0"/>
+      <c r="HQ11" s="0"/>
+      <c r="HR11" s="0"/>
+      <c r="HS11" s="0"/>
+      <c r="HT11" s="0"/>
+      <c r="HU11" s="0"/>
+      <c r="HV11" s="0"/>
+      <c r="HW11" s="0"/>
+      <c r="HX11" s="0"/>
+      <c r="HY11" s="0"/>
+      <c r="HZ11" s="0"/>
+      <c r="IA11" s="0"/>
+      <c r="IB11" s="0"/>
+      <c r="IC11" s="0"/>
+      <c r="ID11" s="0"/>
+      <c r="IE11" s="0"/>
+      <c r="IF11" s="0"/>
+      <c r="IG11" s="0"/>
+      <c r="IH11" s="0"/>
+      <c r="II11" s="0"/>
+      <c r="IJ11" s="0"/>
+      <c r="IK11" s="0"/>
+      <c r="IL11" s="0"/>
+      <c r="IM11" s="0"/>
+      <c r="IN11" s="0"/>
+      <c r="IO11" s="0"/>
+      <c r="IP11" s="0"/>
+      <c r="IQ11" s="0"/>
+      <c r="IR11" s="0"/>
+      <c r="IS11" s="0"/>
+      <c r="IT11" s="0"/>
+      <c r="IU11" s="0"/>
+      <c r="IV11" s="0"/>
+      <c r="IW11" s="0"/>
+      <c r="IX11" s="0"/>
+      <c r="IY11" s="0"/>
+      <c r="IZ11" s="0"/>
+      <c r="JA11" s="0"/>
+      <c r="JB11" s="0"/>
+      <c r="JC11" s="0"/>
+      <c r="JD11" s="0"/>
+      <c r="JE11" s="0"/>
+      <c r="JF11" s="0"/>
+      <c r="JG11" s="0"/>
+      <c r="JH11" s="0"/>
+      <c r="JI11" s="0"/>
+      <c r="JJ11" s="0"/>
+      <c r="JK11" s="0"/>
+      <c r="JL11" s="0"/>
+      <c r="JM11" s="0"/>
+      <c r="JN11" s="0"/>
+      <c r="JO11" s="0"/>
+      <c r="JP11" s="0"/>
+      <c r="JQ11" s="0"/>
+      <c r="JR11" s="0"/>
+      <c r="JS11" s="0"/>
+      <c r="JT11" s="0"/>
+      <c r="JU11" s="0"/>
+      <c r="JV11" s="0"/>
+      <c r="JW11" s="0"/>
+      <c r="JX11" s="0"/>
+      <c r="JY11" s="0"/>
+      <c r="JZ11" s="0"/>
+      <c r="KA11" s="0"/>
+      <c r="KB11" s="0"/>
+      <c r="KC11" s="0"/>
+      <c r="KD11" s="0"/>
+      <c r="KE11" s="0"/>
+      <c r="KF11" s="0"/>
+      <c r="KG11" s="0"/>
+      <c r="KH11" s="0"/>
+      <c r="KI11" s="0"/>
+      <c r="KJ11" s="0"/>
+      <c r="KK11" s="0"/>
+      <c r="KL11" s="0"/>
+      <c r="KM11" s="0"/>
+      <c r="KN11" s="0"/>
+      <c r="KO11" s="0"/>
+      <c r="KP11" s="0"/>
+      <c r="KQ11" s="0"/>
+      <c r="KR11" s="0"/>
+      <c r="KS11" s="0"/>
+      <c r="KT11" s="0"/>
+      <c r="KU11" s="0"/>
+      <c r="KV11" s="0"/>
+      <c r="KW11" s="0"/>
+      <c r="KX11" s="0"/>
+      <c r="KY11" s="0"/>
+      <c r="KZ11" s="0"/>
+      <c r="LA11" s="0"/>
+      <c r="LB11" s="0"/>
+      <c r="LC11" s="0"/>
+      <c r="LD11" s="0"/>
+      <c r="LE11" s="0"/>
+      <c r="LF11" s="0"/>
+      <c r="LG11" s="0"/>
+      <c r="LH11" s="0"/>
+      <c r="LI11" s="0"/>
+      <c r="LJ11" s="0"/>
+      <c r="LK11" s="0"/>
+      <c r="LL11" s="0"/>
+      <c r="LM11" s="0"/>
+      <c r="LN11" s="0"/>
+      <c r="LO11" s="0"/>
+      <c r="LP11" s="0"/>
+      <c r="LQ11" s="0"/>
+      <c r="LR11" s="0"/>
+      <c r="LS11" s="0"/>
+      <c r="LT11" s="0"/>
+      <c r="LU11" s="0"/>
+      <c r="LV11" s="0"/>
+      <c r="LW11" s="0"/>
+      <c r="LX11" s="0"/>
+      <c r="LY11" s="0"/>
+      <c r="LZ11" s="0"/>
+      <c r="MA11" s="0"/>
+      <c r="MB11" s="0"/>
+      <c r="MC11" s="0"/>
+      <c r="MD11" s="0"/>
+      <c r="ME11" s="0"/>
+      <c r="MF11" s="0"/>
+      <c r="MG11" s="0"/>
+      <c r="MH11" s="0"/>
+      <c r="MI11" s="0"/>
+      <c r="MJ11" s="0"/>
+      <c r="MK11" s="0"/>
+      <c r="ML11" s="0"/>
+      <c r="MM11" s="0"/>
+      <c r="MN11" s="0"/>
+      <c r="MO11" s="0"/>
+      <c r="MP11" s="0"/>
+      <c r="MQ11" s="0"/>
+      <c r="MR11" s="0"/>
+      <c r="MS11" s="0"/>
+      <c r="MT11" s="0"/>
+      <c r="MU11" s="0"/>
+      <c r="MV11" s="0"/>
+      <c r="MW11" s="0"/>
+      <c r="MX11" s="0"/>
+      <c r="MY11" s="0"/>
+      <c r="MZ11" s="0"/>
+      <c r="NA11" s="0"/>
+      <c r="NB11" s="0"/>
+      <c r="NC11" s="0"/>
+      <c r="ND11" s="0"/>
+      <c r="NE11" s="0"/>
+      <c r="NF11" s="0"/>
+      <c r="NG11" s="0"/>
+      <c r="NH11" s="0"/>
+      <c r="NI11" s="0"/>
+      <c r="NJ11" s="0"/>
+      <c r="NK11" s="0"/>
+      <c r="NL11" s="0"/>
+      <c r="NM11" s="0"/>
+      <c r="NN11" s="0"/>
+      <c r="NO11" s="0"/>
+      <c r="NP11" s="0"/>
+      <c r="NQ11" s="0"/>
+      <c r="NR11" s="0"/>
+      <c r="NS11" s="0"/>
+      <c r="NT11" s="0"/>
+      <c r="NU11" s="0"/>
+      <c r="NV11" s="0"/>
+      <c r="NW11" s="0"/>
+      <c r="NX11" s="0"/>
+      <c r="NY11" s="0"/>
+      <c r="NZ11" s="0"/>
+      <c r="OA11" s="0"/>
+      <c r="OB11" s="0"/>
+      <c r="OC11" s="0"/>
+      <c r="OD11" s="0"/>
+      <c r="OE11" s="0"/>
+      <c r="OF11" s="0"/>
+      <c r="OG11" s="0"/>
+      <c r="OH11" s="0"/>
+      <c r="OI11" s="0"/>
+      <c r="OJ11" s="0"/>
+      <c r="OK11" s="0"/>
+      <c r="OL11" s="0"/>
+      <c r="OM11" s="0"/>
+      <c r="ON11" s="0"/>
+      <c r="OO11" s="0"/>
+      <c r="OP11" s="0"/>
+      <c r="OQ11" s="0"/>
+      <c r="OR11" s="0"/>
+      <c r="OS11" s="0"/>
+      <c r="OT11" s="0"/>
+      <c r="OU11" s="0"/>
+      <c r="OV11" s="0"/>
+      <c r="OW11" s="0"/>
+      <c r="OX11" s="0"/>
+      <c r="OY11" s="0"/>
+      <c r="OZ11" s="0"/>
+      <c r="PA11" s="0"/>
+      <c r="PB11" s="0"/>
+      <c r="PC11" s="0"/>
+      <c r="PD11" s="0"/>
+      <c r="PE11" s="0"/>
+      <c r="PF11" s="0"/>
+      <c r="PG11" s="0"/>
+      <c r="PH11" s="0"/>
+      <c r="PI11" s="0"/>
+      <c r="PJ11" s="0"/>
+      <c r="PK11" s="0"/>
+      <c r="PL11" s="0"/>
+      <c r="PM11" s="0"/>
+      <c r="PN11" s="0"/>
+      <c r="PO11" s="0"/>
+      <c r="PP11" s="0"/>
+      <c r="PQ11" s="0"/>
+      <c r="PR11" s="0"/>
+      <c r="PS11" s="0"/>
+      <c r="PT11" s="0"/>
+      <c r="PU11" s="0"/>
+      <c r="PV11" s="0"/>
+      <c r="PW11" s="0"/>
+      <c r="PX11" s="0"/>
+      <c r="PY11" s="0"/>
+      <c r="PZ11" s="0"/>
+      <c r="QA11" s="0"/>
+      <c r="QB11" s="0"/>
+      <c r="QC11" s="0"/>
+      <c r="QD11" s="0"/>
+      <c r="QE11" s="0"/>
+      <c r="QF11" s="0"/>
+      <c r="QG11" s="0"/>
+      <c r="QH11" s="0"/>
+      <c r="QI11" s="0"/>
+      <c r="QJ11" s="0"/>
+      <c r="QK11" s="0"/>
+      <c r="QL11" s="0"/>
+      <c r="QM11" s="0"/>
+      <c r="QN11" s="0"/>
+      <c r="QO11" s="0"/>
+      <c r="QP11" s="0"/>
+      <c r="QQ11" s="0"/>
+      <c r="QR11" s="0"/>
+      <c r="QS11" s="0"/>
+      <c r="QT11" s="0"/>
+      <c r="QU11" s="0"/>
+      <c r="QV11" s="0"/>
+      <c r="QW11" s="0"/>
+      <c r="QX11" s="0"/>
+      <c r="QY11" s="0"/>
+      <c r="QZ11" s="0"/>
+      <c r="RA11" s="0"/>
+      <c r="RB11" s="0"/>
+      <c r="RC11" s="0"/>
+      <c r="RD11" s="0"/>
+      <c r="RE11" s="0"/>
+      <c r="RF11" s="0"/>
+      <c r="RG11" s="0"/>
+      <c r="RH11" s="0"/>
+      <c r="RI11" s="0"/>
+      <c r="RJ11" s="0"/>
+      <c r="RK11" s="0"/>
+      <c r="RL11" s="0"/>
+      <c r="RM11" s="0"/>
+      <c r="RN11" s="0"/>
+      <c r="RO11" s="0"/>
+      <c r="RP11" s="0"/>
+      <c r="RQ11" s="0"/>
+      <c r="RR11" s="0"/>
+      <c r="RS11" s="0"/>
+      <c r="RT11" s="0"/>
+      <c r="RU11" s="0"/>
+      <c r="RV11" s="0"/>
+      <c r="RW11" s="0"/>
+      <c r="RX11" s="0"/>
+      <c r="RY11" s="0"/>
+      <c r="RZ11" s="0"/>
+      <c r="SA11" s="0"/>
+      <c r="SB11" s="0"/>
+      <c r="SC11" s="0"/>
+      <c r="SD11" s="0"/>
+      <c r="SE11" s="0"/>
+      <c r="SF11" s="0"/>
+      <c r="SG11" s="0"/>
+      <c r="SH11" s="0"/>
+      <c r="SI11" s="0"/>
+      <c r="SJ11" s="0"/>
+      <c r="SK11" s="0"/>
+      <c r="SL11" s="0"/>
+      <c r="SM11" s="0"/>
+      <c r="SN11" s="0"/>
+      <c r="SO11" s="0"/>
+      <c r="SP11" s="0"/>
+      <c r="SQ11" s="0"/>
+      <c r="SR11" s="0"/>
+      <c r="SS11" s="0"/>
+      <c r="ST11" s="0"/>
+      <c r="SU11" s="0"/>
+      <c r="SV11" s="0"/>
+      <c r="SW11" s="0"/>
+      <c r="SX11" s="0"/>
+      <c r="SY11" s="0"/>
+      <c r="SZ11" s="0"/>
+      <c r="TA11" s="0"/>
+      <c r="TB11" s="0"/>
+      <c r="TC11" s="0"/>
+      <c r="TD11" s="0"/>
+      <c r="TE11" s="0"/>
+      <c r="TF11" s="0"/>
+      <c r="TG11" s="0"/>
+      <c r="TH11" s="0"/>
+      <c r="TI11" s="0"/>
+      <c r="TJ11" s="0"/>
+      <c r="TK11" s="0"/>
+      <c r="TL11" s="0"/>
+      <c r="TM11" s="0"/>
+      <c r="TN11" s="0"/>
+      <c r="TO11" s="0"/>
+      <c r="TP11" s="0"/>
+      <c r="TQ11" s="0"/>
+      <c r="TR11" s="0"/>
+      <c r="TS11" s="0"/>
+      <c r="TT11" s="0"/>
+      <c r="TU11" s="0"/>
+      <c r="TV11" s="0"/>
+      <c r="TW11" s="0"/>
+      <c r="TX11" s="0"/>
+      <c r="TY11" s="0"/>
+      <c r="TZ11" s="0"/>
+      <c r="UA11" s="0"/>
+      <c r="UB11" s="0"/>
+      <c r="UC11" s="0"/>
+      <c r="UD11" s="0"/>
+      <c r="UE11" s="0"/>
+      <c r="UF11" s="0"/>
+      <c r="UG11" s="0"/>
+      <c r="UH11" s="0"/>
+      <c r="UI11" s="0"/>
+      <c r="UJ11" s="0"/>
+      <c r="UK11" s="0"/>
+      <c r="UL11" s="0"/>
+      <c r="UM11" s="0"/>
+      <c r="UN11" s="0"/>
+      <c r="UO11" s="0"/>
+      <c r="UP11" s="0"/>
+      <c r="UQ11" s="0"/>
+      <c r="UR11" s="0"/>
+      <c r="US11" s="0"/>
+      <c r="UT11" s="0"/>
+      <c r="UU11" s="0"/>
+      <c r="UV11" s="0"/>
+      <c r="UW11" s="0"/>
+      <c r="UX11" s="0"/>
+      <c r="UY11" s="0"/>
+      <c r="UZ11" s="0"/>
+      <c r="VA11" s="0"/>
+      <c r="VB11" s="0"/>
+      <c r="VC11" s="0"/>
+      <c r="VD11" s="0"/>
+      <c r="VE11" s="0"/>
+      <c r="VF11" s="0"/>
+      <c r="VG11" s="0"/>
+      <c r="VH11" s="0"/>
+      <c r="VI11" s="0"/>
+      <c r="VJ11" s="0"/>
+      <c r="VK11" s="0"/>
+      <c r="VL11" s="0"/>
+      <c r="VM11" s="0"/>
+      <c r="VN11" s="0"/>
+      <c r="VO11" s="0"/>
+      <c r="VP11" s="0"/>
+      <c r="VQ11" s="0"/>
+      <c r="VR11" s="0"/>
+      <c r="VS11" s="0"/>
+      <c r="VT11" s="0"/>
+      <c r="VU11" s="0"/>
+      <c r="VV11" s="0"/>
+      <c r="VW11" s="0"/>
+      <c r="VX11" s="0"/>
+      <c r="VY11" s="0"/>
+      <c r="VZ11" s="0"/>
+      <c r="WA11" s="0"/>
+      <c r="WB11" s="0"/>
+      <c r="WC11" s="0"/>
+      <c r="WD11" s="0"/>
+      <c r="WE11" s="0"/>
+      <c r="WF11" s="0"/>
+      <c r="WG11" s="0"/>
+      <c r="WH11" s="0"/>
+      <c r="WI11" s="0"/>
+      <c r="WJ11" s="0"/>
+      <c r="WK11" s="0"/>
+      <c r="WL11" s="0"/>
+      <c r="WM11" s="0"/>
+      <c r="WN11" s="0"/>
+      <c r="WO11" s="0"/>
+      <c r="WP11" s="0"/>
+      <c r="WQ11" s="0"/>
+      <c r="WR11" s="0"/>
+      <c r="WS11" s="0"/>
+      <c r="WT11" s="0"/>
+      <c r="WU11" s="0"/>
+      <c r="WV11" s="0"/>
+      <c r="WW11" s="0"/>
+      <c r="WX11" s="0"/>
+      <c r="WY11" s="0"/>
+      <c r="WZ11" s="0"/>
+      <c r="XA11" s="0"/>
+      <c r="XB11" s="0"/>
+      <c r="XC11" s="0"/>
+      <c r="XD11" s="0"/>
+      <c r="XE11" s="0"/>
+      <c r="XF11" s="0"/>
+      <c r="XG11" s="0"/>
+      <c r="XH11" s="0"/>
+      <c r="XI11" s="0"/>
+      <c r="XJ11" s="0"/>
+      <c r="XK11" s="0"/>
+      <c r="XL11" s="0"/>
+      <c r="XM11" s="0"/>
+      <c r="XN11" s="0"/>
+      <c r="XO11" s="0"/>
+      <c r="XP11" s="0"/>
+      <c r="XQ11" s="0"/>
+      <c r="XR11" s="0"/>
+      <c r="XS11" s="0"/>
+      <c r="XT11" s="0"/>
+      <c r="XU11" s="0"/>
+      <c r="XV11" s="0"/>
+      <c r="XW11" s="0"/>
+      <c r="XX11" s="0"/>
+      <c r="XY11" s="0"/>
+      <c r="XZ11" s="0"/>
+      <c r="YA11" s="0"/>
+      <c r="YB11" s="0"/>
+      <c r="YC11" s="0"/>
+      <c r="YD11" s="0"/>
+      <c r="YE11" s="0"/>
+      <c r="YF11" s="0"/>
+      <c r="YG11" s="0"/>
+      <c r="YH11" s="0"/>
+      <c r="YI11" s="0"/>
+      <c r="YJ11" s="0"/>
+      <c r="YK11" s="0"/>
+      <c r="YL11" s="0"/>
+      <c r="YM11" s="0"/>
+      <c r="YN11" s="0"/>
+      <c r="YO11" s="0"/>
+      <c r="YP11" s="0"/>
+      <c r="YQ11" s="0"/>
+      <c r="YR11" s="0"/>
+      <c r="YS11" s="0"/>
+      <c r="YT11" s="0"/>
+      <c r="YU11" s="0"/>
+      <c r="YV11" s="0"/>
+      <c r="YW11" s="0"/>
+      <c r="YX11" s="0"/>
+      <c r="YY11" s="0"/>
+      <c r="YZ11" s="0"/>
+      <c r="ZA11" s="0"/>
+      <c r="ZB11" s="0"/>
+      <c r="ZC11" s="0"/>
+      <c r="ZD11" s="0"/>
+      <c r="ZE11" s="0"/>
+      <c r="ZF11" s="0"/>
+      <c r="ZG11" s="0"/>
+      <c r="ZH11" s="0"/>
+      <c r="ZI11" s="0"/>
+      <c r="ZJ11" s="0"/>
+      <c r="ZK11" s="0"/>
+      <c r="ZL11" s="0"/>
+      <c r="ZM11" s="0"/>
+      <c r="ZN11" s="0"/>
+      <c r="ZO11" s="0"/>
+      <c r="ZP11" s="0"/>
+      <c r="ZQ11" s="0"/>
+      <c r="ZR11" s="0"/>
+      <c r="ZS11" s="0"/>
+      <c r="ZT11" s="0"/>
+      <c r="ZU11" s="0"/>
+      <c r="ZV11" s="0"/>
+      <c r="ZW11" s="0"/>
+      <c r="ZX11" s="0"/>
+      <c r="ZY11" s="0"/>
+      <c r="ZZ11" s="0"/>
+      <c r="AAA11" s="0"/>
+      <c r="AAB11" s="0"/>
+      <c r="AAC11" s="0"/>
+      <c r="AAD11" s="0"/>
+      <c r="AAE11" s="0"/>
+      <c r="AAF11" s="0"/>
+      <c r="AAG11" s="0"/>
+      <c r="AAH11" s="0"/>
+      <c r="AAI11" s="0"/>
+      <c r="AAJ11" s="0"/>
+      <c r="AAK11" s="0"/>
+      <c r="AAL11" s="0"/>
+      <c r="AAM11" s="0"/>
+      <c r="AAN11" s="0"/>
+      <c r="AAO11" s="0"/>
+      <c r="AAP11" s="0"/>
+      <c r="AAQ11" s="0"/>
+      <c r="AAR11" s="0"/>
+      <c r="AAS11" s="0"/>
+      <c r="AAT11" s="0"/>
+      <c r="AAU11" s="0"/>
+      <c r="AAV11" s="0"/>
+      <c r="AAW11" s="0"/>
+      <c r="AAX11" s="0"/>
+      <c r="AAY11" s="0"/>
+      <c r="AAZ11" s="0"/>
+      <c r="ABA11" s="0"/>
+      <c r="ABB11" s="0"/>
+      <c r="ABC11" s="0"/>
+      <c r="ABD11" s="0"/>
+      <c r="ABE11" s="0"/>
+      <c r="ABF11" s="0"/>
+      <c r="ABG11" s="0"/>
+      <c r="ABH11" s="0"/>
+      <c r="ABI11" s="0"/>
+      <c r="ABJ11" s="0"/>
+      <c r="ABK11" s="0"/>
+      <c r="ABL11" s="0"/>
+      <c r="ABM11" s="0"/>
+      <c r="ABN11" s="0"/>
+      <c r="ABO11" s="0"/>
+      <c r="ABP11" s="0"/>
+      <c r="ABQ11" s="0"/>
+      <c r="ABR11" s="0"/>
+      <c r="ABS11" s="0"/>
+      <c r="ABT11" s="0"/>
+      <c r="ABU11" s="0"/>
+      <c r="ABV11" s="0"/>
+      <c r="ABW11" s="0"/>
+      <c r="ABX11" s="0"/>
+      <c r="ABY11" s="0"/>
+      <c r="ABZ11" s="0"/>
+      <c r="ACA11" s="0"/>
+      <c r="ACB11" s="0"/>
+      <c r="ACC11" s="0"/>
+      <c r="ACD11" s="0"/>
+      <c r="ACE11" s="0"/>
+      <c r="ACF11" s="0"/>
+      <c r="ACG11" s="0"/>
+      <c r="ACH11" s="0"/>
+      <c r="ACI11" s="0"/>
+      <c r="ACJ11" s="0"/>
+      <c r="ACK11" s="0"/>
+      <c r="ACL11" s="0"/>
+      <c r="ACM11" s="0"/>
+      <c r="ACN11" s="0"/>
+      <c r="ACO11" s="0"/>
+      <c r="ACP11" s="0"/>
+      <c r="ACQ11" s="0"/>
+      <c r="ACR11" s="0"/>
+      <c r="ACS11" s="0"/>
+      <c r="ACT11" s="0"/>
+      <c r="ACU11" s="0"/>
+      <c r="ACV11" s="0"/>
+      <c r="ACW11" s="0"/>
+      <c r="ACX11" s="0"/>
+      <c r="ACY11" s="0"/>
+      <c r="ACZ11" s="0"/>
+      <c r="ADA11" s="0"/>
+      <c r="ADB11" s="0"/>
+      <c r="ADC11" s="0"/>
+      <c r="ADD11" s="0"/>
+      <c r="ADE11" s="0"/>
+      <c r="ADF11" s="0"/>
+      <c r="ADG11" s="0"/>
+      <c r="ADH11" s="0"/>
+      <c r="ADI11" s="0"/>
+      <c r="ADJ11" s="0"/>
+      <c r="ADK11" s="0"/>
+      <c r="ADL11" s="0"/>
+      <c r="ADM11" s="0"/>
+      <c r="ADN11" s="0"/>
+      <c r="ADO11" s="0"/>
+      <c r="ADP11" s="0"/>
+      <c r="ADQ11" s="0"/>
+      <c r="ADR11" s="0"/>
+      <c r="ADS11" s="0"/>
+      <c r="ADT11" s="0"/>
+      <c r="ADU11" s="0"/>
+      <c r="ADV11" s="0"/>
+      <c r="ADW11" s="0"/>
+      <c r="ADX11" s="0"/>
+      <c r="ADY11" s="0"/>
+      <c r="ADZ11" s="0"/>
+      <c r="AEA11" s="0"/>
+      <c r="AEB11" s="0"/>
+      <c r="AEC11" s="0"/>
+      <c r="AED11" s="0"/>
+      <c r="AEE11" s="0"/>
+      <c r="AEF11" s="0"/>
+      <c r="AEG11" s="0"/>
+      <c r="AEH11" s="0"/>
+      <c r="AEI11" s="0"/>
+      <c r="AEJ11" s="0"/>
+      <c r="AEK11" s="0"/>
+      <c r="AEL11" s="0"/>
+      <c r="AEM11" s="0"/>
+      <c r="AEN11" s="0"/>
+      <c r="AEO11" s="0"/>
+      <c r="AEP11" s="0"/>
+      <c r="AEQ11" s="0"/>
+      <c r="AER11" s="0"/>
+      <c r="AES11" s="0"/>
+      <c r="AET11" s="0"/>
+      <c r="AEU11" s="0"/>
+      <c r="AEV11" s="0"/>
+      <c r="AEW11" s="0"/>
+      <c r="AEX11" s="0"/>
+      <c r="AEY11" s="0"/>
+      <c r="AEZ11" s="0"/>
+      <c r="AFA11" s="0"/>
+      <c r="AFB11" s="0"/>
+      <c r="AFC11" s="0"/>
+      <c r="AFD11" s="0"/>
+      <c r="AFE11" s="0"/>
+      <c r="AFF11" s="0"/>
+      <c r="AFG11" s="0"/>
+      <c r="AFH11" s="0"/>
+      <c r="AFI11" s="0"/>
+      <c r="AFJ11" s="0"/>
+      <c r="AFK11" s="0"/>
+      <c r="AFL11" s="0"/>
+      <c r="AFM11" s="0"/>
+      <c r="AFN11" s="0"/>
+      <c r="AFO11" s="0"/>
+      <c r="AFP11" s="0"/>
+      <c r="AFQ11" s="0"/>
+      <c r="AFR11" s="0"/>
+      <c r="AFS11" s="0"/>
+      <c r="AFT11" s="0"/>
+      <c r="AFU11" s="0"/>
+      <c r="AFV11" s="0"/>
+      <c r="AFW11" s="0"/>
+      <c r="AFX11" s="0"/>
+      <c r="AFY11" s="0"/>
+      <c r="AFZ11" s="0"/>
+      <c r="AGA11" s="0"/>
+      <c r="AGB11" s="0"/>
+      <c r="AGC11" s="0"/>
+      <c r="AGD11" s="0"/>
+      <c r="AGE11" s="0"/>
+      <c r="AGF11" s="0"/>
+      <c r="AGG11" s="0"/>
+      <c r="AGH11" s="0"/>
+      <c r="AGI11" s="0"/>
+      <c r="AGJ11" s="0"/>
+      <c r="AGK11" s="0"/>
+      <c r="AGL11" s="0"/>
+      <c r="AGM11" s="0"/>
+      <c r="AGN11" s="0"/>
+      <c r="AGO11" s="0"/>
+      <c r="AGP11" s="0"/>
+      <c r="AGQ11" s="0"/>
+      <c r="AGR11" s="0"/>
+      <c r="AGS11" s="0"/>
+      <c r="AGT11" s="0"/>
+      <c r="AGU11" s="0"/>
+      <c r="AGV11" s="0"/>
+      <c r="AGW11" s="0"/>
+      <c r="AGX11" s="0"/>
+      <c r="AGY11" s="0"/>
+      <c r="AGZ11" s="0"/>
+      <c r="AHA11" s="0"/>
+      <c r="AHB11" s="0"/>
+      <c r="AHC11" s="0"/>
+      <c r="AHD11" s="0"/>
+      <c r="AHE11" s="0"/>
+      <c r="AHF11" s="0"/>
+      <c r="AHG11" s="0"/>
+      <c r="AHH11" s="0"/>
+      <c r="AHI11" s="0"/>
+      <c r="AHJ11" s="0"/>
+      <c r="AHK11" s="0"/>
+      <c r="AHL11" s="0"/>
+      <c r="AHM11" s="0"/>
+      <c r="AHN11" s="0"/>
+      <c r="AHO11" s="0"/>
+      <c r="AHP11" s="0"/>
+      <c r="AHQ11" s="0"/>
+      <c r="AHR11" s="0"/>
+      <c r="AHS11" s="0"/>
+      <c r="AHT11" s="0"/>
+      <c r="AHU11" s="0"/>
+      <c r="AHV11" s="0"/>
+      <c r="AHW11" s="0"/>
+      <c r="AHX11" s="0"/>
+      <c r="AHY11" s="0"/>
+      <c r="AHZ11" s="0"/>
+      <c r="AIA11" s="0"/>
+      <c r="AIB11" s="0"/>
+      <c r="AIC11" s="0"/>
+      <c r="AID11" s="0"/>
+      <c r="AIE11" s="0"/>
+      <c r="AIF11" s="0"/>
+      <c r="AIG11" s="0"/>
+      <c r="AIH11" s="0"/>
+      <c r="AII11" s="0"/>
+      <c r="AIJ11" s="0"/>
+      <c r="AIK11" s="0"/>
+      <c r="AIL11" s="0"/>
+      <c r="AIM11" s="0"/>
+      <c r="AIN11" s="0"/>
+      <c r="AIO11" s="0"/>
+      <c r="AIP11" s="0"/>
+      <c r="AIQ11" s="0"/>
+      <c r="AIR11" s="0"/>
+      <c r="AIS11" s="0"/>
+      <c r="AIT11" s="0"/>
+      <c r="AIU11" s="0"/>
+      <c r="AIV11" s="0"/>
+      <c r="AIW11" s="0"/>
+      <c r="AIX11" s="0"/>
+      <c r="AIY11" s="0"/>
+      <c r="AIZ11" s="0"/>
+      <c r="AJA11" s="0"/>
+      <c r="AJB11" s="0"/>
+      <c r="AJC11" s="0"/>
+      <c r="AJD11" s="0"/>
+      <c r="AJE11" s="0"/>
+      <c r="AJF11" s="0"/>
+      <c r="AJG11" s="0"/>
+      <c r="AJH11" s="0"/>
+      <c r="AJI11" s="0"/>
+      <c r="AJJ11" s="0"/>
+      <c r="AJK11" s="0"/>
+      <c r="AJL11" s="0"/>
+      <c r="AJM11" s="0"/>
+      <c r="AJN11" s="0"/>
+      <c r="AJO11" s="0"/>
+      <c r="AJP11" s="0"/>
+      <c r="AJQ11" s="0"/>
+      <c r="AJR11" s="0"/>
+      <c r="AJS11" s="0"/>
+      <c r="AJT11" s="0"/>
+      <c r="AJU11" s="0"/>
+      <c r="AJV11" s="0"/>
+      <c r="AJW11" s="0"/>
+      <c r="AJX11" s="0"/>
+      <c r="AJY11" s="0"/>
+      <c r="AJZ11" s="0"/>
+      <c r="AKA11" s="0"/>
+      <c r="AKB11" s="0"/>
+      <c r="AKC11" s="0"/>
+      <c r="AKD11" s="0"/>
+      <c r="AKE11" s="0"/>
+      <c r="AKF11" s="0"/>
+      <c r="AKG11" s="0"/>
+      <c r="AKH11" s="0"/>
+      <c r="AKI11" s="0"/>
+      <c r="AKJ11" s="0"/>
+      <c r="AKK11" s="0"/>
+      <c r="AKL11" s="0"/>
+      <c r="AKM11" s="0"/>
+      <c r="AKN11" s="0"/>
+      <c r="AKO11" s="0"/>
+      <c r="AKP11" s="0"/>
+      <c r="AKQ11" s="0"/>
+      <c r="AKR11" s="0"/>
+      <c r="AKS11" s="0"/>
+      <c r="AKT11" s="0"/>
+      <c r="AKU11" s="0"/>
+      <c r="AKV11" s="0"/>
+      <c r="AKW11" s="0"/>
+      <c r="AKX11" s="0"/>
+      <c r="AKY11" s="0"/>
+      <c r="AKZ11" s="0"/>
+      <c r="ALA11" s="0"/>
+      <c r="ALB11" s="0"/>
+      <c r="ALC11" s="0"/>
+      <c r="ALD11" s="0"/>
+      <c r="ALE11" s="0"/>
+      <c r="ALF11" s="0"/>
+      <c r="ALG11" s="0"/>
+      <c r="ALH11" s="0"/>
+      <c r="ALI11" s="0"/>
+      <c r="ALJ11" s="0"/>
+      <c r="ALK11" s="0"/>
+      <c r="ALL11" s="0"/>
+      <c r="ALM11" s="0"/>
+      <c r="ALN11" s="0"/>
+      <c r="ALO11" s="0"/>
+      <c r="ALP11" s="0"/>
+      <c r="ALQ11" s="0"/>
+      <c r="ALR11" s="0"/>
+      <c r="ALS11" s="0"/>
+      <c r="ALT11" s="0"/>
+      <c r="ALU11" s="0"/>
+      <c r="ALV11" s="0"/>
+      <c r="ALW11" s="0"/>
+      <c r="ALX11" s="0"/>
+      <c r="ALY11" s="0"/>
+      <c r="ALZ11" s="0"/>
+      <c r="AMA11" s="0"/>
+      <c r="AMB11" s="0"/>
+      <c r="AMC11" s="0"/>
+      <c r="AMD11" s="0"/>
+      <c r="AME11" s="0"/>
+      <c r="AMF11" s="0"/>
+      <c r="AMG11" s="0"/>
+      <c r="AMH11" s="0"/>
+      <c r="AMI11" s="0"/>
+      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>26</v>
@@ -11364,14 +12382,14 @@
         <v>26</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="7" t="n">
@@ -11382,7 +12400,7 @@
     <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>26</v>
@@ -11391,7 +12409,7 @@
         <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>18</v>
@@ -11406,57 +12424,59 @@
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="7" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8" t="n">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="J14" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="7"/>
+      <c r="K14" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="I15" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="I15" s="3"/>
       <c r="J15" s="3" t="n">
         <v>0</v>
       </c>
@@ -11465,89 +12485,60 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5" t="s">
-        <v>33</v>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3" t="n">
-        <v>16</v>
+      <c r="H16" s="4" t="n">
+        <v>0.8</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="4" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3" t="n">
         <v>10</v>
       </c>
       <c r="K17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="K18" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -11573,14 +12564,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="6.3469387755102"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="10" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="10" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="10" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11590,7 +12581,7 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
       <c r="F1" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
@@ -11604,37 +12595,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3" s="17" t="n">
         <v>390</v>
@@ -11652,10 +12643,10 @@
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" s="19" t="n">
         <v>9555589203096</v>
@@ -11675,10 +12666,10 @@
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="19" t="n">
         <v>9555589203287</v>
@@ -11698,10 +12689,10 @@
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="19" t="n">
         <v>9555589200415</v>
@@ -11723,10 +12714,10 @@
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" s="19" t="n">
         <v>9555589203348</v>
@@ -11748,10 +12739,10 @@
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" s="19" t="n">
         <v>9555589200385</v>
@@ -11773,14 +12764,14 @@
     </row>
     <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E9" s="17" t="n">
         <v>390</v>
@@ -11800,14 +12791,14 @@
     </row>
     <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E10" s="17" t="n">
         <v>1.25</v>
@@ -11827,10 +12818,10 @@
     </row>
     <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="19" t="n">
         <v>9555589203294</v>
@@ -11852,10 +12843,10 @@
     </row>
     <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="19" t="n">
         <v>9555589203102</v>
@@ -11877,14 +12868,14 @@
     </row>
     <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E13" s="17" t="n">
         <v>315</v>
@@ -11904,14 +12895,14 @@
     </row>
     <row r="14" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" s="17" t="n">
         <v>350</v>
@@ -11931,14 +12922,14 @@
     </row>
     <row r="15" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" s="17" t="n">
         <v>500</v>
@@ -11952,14 +12943,14 @@
     </row>
     <row r="16" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" s="17" t="n">
         <v>1.5</v>
@@ -11973,14 +12964,14 @@
     </row>
     <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E17" s="17" t="n">
         <v>1</v>
@@ -11994,10 +12985,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="23" t="n">
         <v>9555589203287</v>
@@ -12017,10 +13008,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="23" t="n">
         <v>9555589200385</v>
@@ -12040,10 +13031,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" s="23" t="n">
         <v>9555589203096</v>
@@ -12063,10 +13054,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C21" s="23" t="n">
         <v>9555589203294</v>
@@ -12086,10 +13077,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="23" t="n">
         <v>9555589200668</v>
@@ -12109,14 +13100,14 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23" s="18" t="n">
         <v>390</v>
@@ -12134,10 +13125,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C24" s="23" t="n">
         <v>8888002087005</v>
@@ -12157,10 +13148,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" s="23" t="n">
         <v>9555589200415</v>
@@ -12180,10 +13171,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C26" s="23" t="n">
         <v>9555589203102</v>
@@ -12203,14 +13194,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E27" s="18" t="n">
         <v>390</v>
@@ -12228,14 +13219,14 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E28" s="18" t="n">
         <v>1.25</v>
@@ -12249,10 +13240,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C29" s="23" t="n">
         <v>9555589200392</v>
@@ -12268,14 +13259,14 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E30" s="18" t="n">
         <v>315</v>
@@ -12293,14 +13284,14 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E31" s="18" t="n">
         <v>350</v>
@@ -12318,14 +13309,14 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E32" s="18" t="n">
         <v>500</v>
@@ -12339,10 +13330,10 @@
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C33" s="24" t="n">
         <v>9555589200385</v>
@@ -12363,10 +13354,10 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C34" s="26" t="n">
         <v>9555589200668</v>
@@ -12387,14 +13378,14 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E35" s="18" t="n">
         <v>330</v>
@@ -12413,14 +13404,14 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E36" s="18" t="n">
         <v>315</v>
@@ -12439,14 +13430,14 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E37" s="18" t="n">
         <v>350</v>
@@ -12465,14 +13456,14 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E38" s="18" t="n">
         <v>330</v>
@@ -12487,10 +13478,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" s="27" t="n">
         <v>8888002087005</v>
@@ -12507,10 +13498,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C40" s="23" t="n">
         <v>9555589200415</v>
@@ -12526,10 +13517,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" s="23" t="n">
         <v>9555589200699</v>
@@ -12545,10 +13536,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C42" s="23" t="n">
         <v>9555589200392</v>
@@ -12564,10 +13555,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C43" s="23" t="n">
         <v>9555589200385</v>
@@ -12583,14 +13574,14 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E44" s="18" t="n">
         <v>1.5</v>
@@ -12604,10 +13595,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C45" s="23" t="n">
         <v>9555589200644</v>
@@ -12623,14 +13614,14 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E46" s="18" t="n">
         <v>1.5</v>
@@ -12644,10 +13635,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C47" s="23" t="n">
         <v>9555589200675</v>
@@ -12663,10 +13654,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C48" s="23" t="n">
         <v>9555589200637</v>
@@ -12682,14 +13673,14 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E49" s="18" t="n">
         <v>500</v>
@@ -12703,14 +13694,14 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E50" s="18" t="n">
         <v>500</v>
@@ -12724,14 +13715,14 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E51" s="18" t="n">
         <v>500</v>
@@ -12745,14 +13736,14 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C52" s="23"/>
       <c r="D52" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E52" s="18" t="n">
         <v>350</v>
@@ -12766,14 +13757,14 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C53" s="23"/>
       <c r="D53" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E53" s="18" t="n">
         <v>1.5</v>
@@ -12787,14 +13778,14 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C54" s="23"/>
       <c r="D54" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E54" s="18" t="n">
         <v>1</v>
@@ -12808,10 +13799,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C55" s="23" t="n">
         <v>9555589203287</v>
@@ -12827,10 +13818,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C56" s="23" t="n">
         <v>9555589200415</v>
@@ -12846,10 +13837,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C57" s="23" t="n">
         <v>9555589203096</v>
@@ -12865,10 +13856,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C58" s="23" t="n">
         <v>9555589203102</v>
@@ -12884,14 +13875,14 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C59" s="23"/>
       <c r="D59" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E59" s="18" t="n">
         <v>1.25</v>
@@ -12905,10 +13896,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C60" s="23" t="n">
         <v>9555589203348</v>
@@ -12924,10 +13915,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C61" s="23" t="n">
         <v>9555589203294</v>
@@ -12943,14 +13934,14 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E62" s="18" t="n">
         <v>500</v>
@@ -12964,10 +13955,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C63" s="23" t="n">
         <v>9555589200385</v>
@@ -12983,14 +13974,14 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C64" s="23"/>
       <c r="D64" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E64" s="18" t="n">
         <v>390</v>
@@ -13004,14 +13995,14 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C65" s="23"/>
       <c r="D65" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E65" s="18" t="n">
         <v>1.25</v>
@@ -13025,14 +14016,14 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C66" s="23"/>
       <c r="D66" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E66" s="18" t="n">
         <v>1.5</v>
@@ -13046,14 +14037,14 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C67" s="23"/>
       <c r="D67" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E67" s="18" t="n">
         <v>1</v>
@@ -13067,14 +14058,14 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C68" s="23"/>
       <c r="D68" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E68" s="18" t="n">
         <v>350</v>
@@ -13088,14 +14079,14 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C69" s="23"/>
       <c r="D69" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E69" s="18" t="n">
         <v>500</v>
@@ -13109,10 +14100,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C70" s="23" t="n">
         <v>9555589200415</v>
@@ -13128,10 +14119,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C71" s="23" t="n">
         <v>9555589200392</v>
@@ -13147,14 +14138,14 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C72" s="23"/>
       <c r="D72" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E72" s="18" t="n">
         <v>500</v>
@@ -13168,10 +14159,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C73" s="23" t="n">
         <v>9555589200699</v>
@@ -13187,10 +14178,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C74" s="23" t="n">
         <v>9555589200644</v>
@@ -13206,14 +14197,14 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C75" s="23"/>
       <c r="D75" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E75" s="18" t="n">
         <v>1.5</v>
@@ -13227,10 +14218,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C76" s="23" t="n">
         <v>9555589200675</v>
@@ -13246,14 +14237,14 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C77" s="23"/>
       <c r="D77" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E77" s="18" t="n">
         <v>500</v>
@@ -13267,14 +14258,14 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C78" s="23"/>
       <c r="D78" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E78" s="18" t="n">
         <v>500</v>
@@ -13288,10 +14279,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C79" s="23" t="n">
         <v>8888002087470</v>
@@ -13307,10 +14298,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C80" s="23" t="n">
         <v>9555589200385</v>
@@ -13326,14 +14317,14 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E81" s="18" t="n">
         <v>500</v>
@@ -13347,14 +14338,14 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C82" s="23"/>
       <c r="D82" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E82" s="18" t="n">
         <v>1.5</v>
@@ -13368,14 +14359,14 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C83" s="23"/>
       <c r="D83" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E83" s="18" t="n">
         <v>1</v>
@@ -13389,14 +14380,14 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C84" s="23"/>
       <c r="D84" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E84" s="18" t="n">
         <v>350</v>
@@ -13410,10 +14401,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C85" s="23" t="n">
         <v>9555589200415</v>
@@ -13429,10 +14420,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C86" s="23" t="n">
         <v>9555589200392</v>
@@ -13448,10 +14439,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C87" s="23" t="n">
         <v>9555589200385</v>
@@ -13467,10 +14458,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C88" s="23" t="n">
         <v>9555589200637</v>
@@ -13486,10 +14477,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="B89" s="18" t="s">
-        <v>96</v>
       </c>
       <c r="C89" s="23" t="n">
         <v>8888002087470</v>
@@ -13505,10 +14496,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C90" s="23" t="n">
         <v>9555589200316</v>
@@ -13524,14 +14515,14 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B91" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C91" s="23"/>
       <c r="D91" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E91" s="18" t="n">
         <v>500</v>
@@ -13545,10 +14536,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C92" s="23" t="n">
         <v>9555589200521</v>
@@ -13564,14 +14555,14 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C93" s="23"/>
       <c r="D93" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E93" s="18" t="n">
         <v>500</v>
@@ -13585,10 +14576,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C94" s="23" t="n">
         <v>9555589200675</v>
@@ -13604,14 +14595,14 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C95" s="23"/>
       <c r="D95" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E95" s="18" t="n">
         <v>500</v>
@@ -13625,10 +14616,10 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C96" s="23" t="n">
         <v>9555589200620</v>
@@ -13644,14 +14635,14 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C97" s="23"/>
       <c r="D97" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E97" s="18" t="n">
         <v>350</v>
@@ -13665,14 +14656,14 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C98" s="23"/>
       <c r="D98" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E98" s="18" t="n">
         <v>1</v>
@@ -13686,14 +14677,14 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C99" s="23"/>
       <c r="D99" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E99" s="18" t="n">
         <v>500</v>

</xml_diff>